<commit_message>
Enhance initial concentration table and worksheet formatting
- Expanded initial concentration table to include "Reagent", "Initial Conc.", and "Units" columns
- Centered all text and added a medium border around the initial concentration block for improved appearance
- Improved header and border styling for main and additional reagents tables
- Refined layout and visual separation for
</commit_message>
<xml_diff>
--- a/mixture_and_component_counts.xlsx
+++ b/mixture_and_component_counts.xlsx
@@ -45,7 +45,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -59,11 +59,69 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -72,6 +130,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1245,7 +1336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1253,90 +1344,220 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Initial Conc. hUba1 (uM)</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Initial Conc. TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Initial Conc. ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5">
+      <c r="D5" s="4" t="inlineStr">
         <is>
           <t>Component</t>
         </is>
       </c>
-      <c r="B1">
+      <c r="E5" s="5">
         <f>'Component Counts'!A2</f>
         <v/>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="7" t="inlineStr">
         <is>
           <t>Component Volume (uL)</t>
         </is>
       </c>
-      <c r="B2">
-        <f>'Component Counts'!C2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="E6" s="8">
+        <f>'Component Counts'!D2</f>
+        <v/>
+      </c>
+      <c r="F6" s="9" t="n"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="7" t="inlineStr">
         <is>
           <t>Amount Needed (nmol)</t>
         </is>
       </c>
-      <c r="B3">
-        <f>'Component Counts'!E2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Stock Conc. 1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Stock Volume 1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Stock Conc. 2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Stock Volume 2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="E7" s="8">
+        <f>'Component Counts'!F2</f>
+        <v/>
+      </c>
+      <c r="F7" s="9" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Stock Conc. 3</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>Stock Conc. 1 (uM)</t>
+        </is>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>Stock Volume 3</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>Stock Volume 1 (uL)</t>
+        </is>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="9">
+        <f>IF(AND(E8&gt;0,E7&gt;0),MIN(E9,ROUND(E7*1000/E8,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>Stock Conc. 2 (uM)</t>
+        </is>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="n"/>
+    </row>
+    <row r="11">
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>Stock Volume 2 (uL)</t>
+        </is>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <f>IF(AND(E10&gt;0,MAX(0,E7-F9*E8/1000)&gt;0),MIN(E11,ROUND(MAX(0,E7-F9*E8/1000)*1000/E10,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>Stock Conc. 3 (uM)</t>
+        </is>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9" t="n"/>
+    </row>
+    <row r="13">
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>Stock Volume 3 (uL)</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <f>IF(AND(E12&gt;0,MAX(0,E7-F9*E8/1000-F11*E10/1000)&gt;0),MIN(G13,ROUND(MAX(0,E7-F9*E8/1000-F11*E10/1000)*1000/E12,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="7" t="inlineStr">
+        <is>
+          <t>Required nmol needed</t>
+        </is>
+      </c>
+      <c r="E14" s="8">
+        <f>ROUND(MAX(0,E7-F9*E8/1000-F11*E10/1000-F13*E12/1000),2)</f>
+        <v/>
+      </c>
+      <c r="F14" s="9" t="n"/>
+    </row>
+    <row r="15">
+      <c r="D15" s="10" t="n"/>
+      <c r="F15" s="9" t="n"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="11" t="inlineStr">
+        <is>
+          <t>Reagent</t>
+        </is>
+      </c>
+      <c r="E16" s="12" t="inlineStr">
+        <is>
+          <t>Final Conc.</t>
+        </is>
+      </c>
+      <c r="F16" s="13" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="11" t="inlineStr">
+        <is>
+          <t>hUba1 (uM)</t>
+        </is>
+      </c>
+      <c r="E17" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="11" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="E18" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="14" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="E19" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F19" s="16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Enhance Base Reagent Prep worksheet: add vertical and horizontal table layout
- Generate 3 vertically stacked Base Reagent Prep tables for Ubc13/Mms2, gp78/Ube2g2, and Ube2K in the left column.
- Add 5 additional tables to the right for ubi_ubq_1_K48_ABOC_K63_ABOC, ubi_ubq_1_K48_SMAC_K63_ABOC, ubi_ubq_1_K48_ABOC_K63_SMAC, ubi_ubq_1_K48_SMAC, and ubi_ubq_1_K63_SMAC.
- Update table placement logic and coordinates for improved worksheet usability and clarity.
- No changes to other worksheet logic or formulas.
</commit_message>
<xml_diff>
--- a/mixture_and_component_counts.xlsx
+++ b/mixture_and_component_counts.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,6 +30,7 @@
     <font>
       <b val="1"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -45,7 +46,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -60,26 +61,34 @@
       <bottom style="thin"/>
     </border>
     <border>
-      <right style="thin"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left style="medium"/>
-      <right style="thin"/>
+      <right/>
       <top style="medium"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <top style="medium"/>
+      <bottom style="medium"/>
     </border>
     <border>
       <left/>
       <right style="medium"/>
       <top style="medium"/>
-      <bottom/>
+      <bottom style="medium"/>
     </border>
     <border>
       <left style="medium"/>
-      <right style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left/>
@@ -91,19 +100,35 @@
       <left style="medium"/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium"/>
     </border>
     <border>
-      <left style="thin"/>
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="medium"/>
+    </border>
+    <border>
       <right style="thin"/>
-      <top/>
-      <bottom/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <bottom style="medium"/>
     </border>
     <border>
       <left style="medium"/>
-      <right/>
-      <top/>
+      <right style="thin"/>
+      <top style="medium"/>
       <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
     </border>
     <border>
       <left style="thin"/>
@@ -112,16 +137,16 @@
       <bottom style="medium"/>
     </border>
     <border>
-      <left/>
-      <right style="medium"/>
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
-      <bottom style="medium"/>
+      <bottom/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -130,37 +155,54 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1336,7 +1378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="B1:L89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1344,221 +1386,1520 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="5" max="5"/>
     <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="23" customWidth="1" min="7" max="7"/>
+    <col width="23" customWidth="1" min="10" max="10"/>
+    <col width="23" customWidth="1" min="11" max="11"/>
+    <col width="23" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Initial Conc. hUba1 (uM)</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr"/>
-    </row>
+    <row r="1"/>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Initial Conc. TCEP (mM)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Initial Conc.</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="n"/>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="F2" s="7">
+        <f>'Component Counts'!A2</f>
+        <v/>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+      <c r="J2" s="6" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="K2" s="7">
+        <f>'Component Counts'!A5</f>
+        <v/>
+      </c>
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>hUba1 (uM)</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Initial Conc. ATP/Mg2+ (mM)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+      <c r="E3" s="10" t="inlineStr">
+        <is>
+          <t>Component Volume (uL)</t>
+        </is>
+      </c>
+      <c r="F3" s="11">
+        <f>'Component Counts'!D2</f>
+        <v/>
+      </c>
+      <c r="G3" s="12" t="n"/>
+      <c r="J3" s="10" t="inlineStr">
+        <is>
+          <t>Component Volume (uL)</t>
+        </is>
+      </c>
+      <c r="K3" s="11">
+        <f>'Component Counts'!D5</f>
+        <v/>
+      </c>
+      <c r="L3" s="12" t="n"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10" t="inlineStr">
+        <is>
+          <t>Amount Needed (nmol)</t>
+        </is>
+      </c>
+      <c r="F4" s="11">
+        <f>'Component Counts'!F2</f>
+        <v/>
+      </c>
+      <c r="G4" s="12" t="n"/>
+      <c r="J4" s="10" t="inlineStr">
+        <is>
+          <t>Amount Needed (nmol)</t>
+        </is>
+      </c>
+      <c r="K4" s="11">
+        <f>'Component Counts'!F5</f>
+        <v/>
+      </c>
+      <c r="L4" s="12" t="n"/>
+    </row>
+    <row r="5">
+      <c r="B5" s="13" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="C5" s="14" t="n">
         <v>100</v>
       </c>
-    </row>
-    <row r="4"/>
-    <row r="5">
-      <c r="D5" s="4" t="inlineStr">
+      <c r="E5" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 1 (uM)</t>
+        </is>
+      </c>
+      <c r="F5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12" t="n"/>
+      <c r="J5" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 1 (uM)</t>
+        </is>
+      </c>
+      <c r="K5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12" t="n"/>
+    </row>
+    <row r="6">
+      <c r="E6" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 1 (uL)</t>
+        </is>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12">
+        <f>IF(AND(F5&gt;0,F4&gt;0),MIN(F6,ROUND(F4*1000/F5,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J6" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 1 (uL)</t>
+        </is>
+      </c>
+      <c r="K6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <f>IF(AND(K5&gt;0,K4&gt;0),MIN(K6,ROUND(K4*1000/K5,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="E7" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 2 (uM)</t>
+        </is>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12" t="n"/>
+      <c r="J7" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 2 (uM)</t>
+        </is>
+      </c>
+      <c r="K7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="12" t="n"/>
+    </row>
+    <row r="8">
+      <c r="E8" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 2 (uL)</t>
+        </is>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <f>IF(AND(F7&gt;0,MAX(0,F4-G6*F5/1000)&gt;0),MIN(F8,ROUND(MAX(0,F4-G6*F5/1000)*1000/F7,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J8" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 2 (uL)</t>
+        </is>
+      </c>
+      <c r="K8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <f>IF(AND(K7&gt;0,MAX(0,K4-L6*K5/1000)&gt;0),MIN(K8,ROUND(MAX(0,K4-L6*K5/1000)*1000/K7,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="E9" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 3 (uM)</t>
+        </is>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12" t="n"/>
+      <c r="J9" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 3 (uM)</t>
+        </is>
+      </c>
+      <c r="K9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12" t="n"/>
+    </row>
+    <row r="10">
+      <c r="E10" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 3 (uL)</t>
+        </is>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="12">
+        <f>IF(AND(F9&gt;0,MAX(0,F4-G6*F5/1000-G8*F7/1000)&gt;0),MIN(H10,ROUND(MAX(0,F4-G6*F5/1000-G8*F7/1000)*1000/F9,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J10" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 3 (uL)</t>
+        </is>
+      </c>
+      <c r="K10" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <f>IF(AND(K9&gt;0,MAX(0,K4-L6*K5/1000-L8*K7/1000)&gt;0),MIN(M10,ROUND(MAX(0,K4-L6*K5/1000-L8*K7/1000)*1000/K9,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="E11" s="10" t="inlineStr">
+        <is>
+          <t>Required nmol needed</t>
+        </is>
+      </c>
+      <c r="F11" s="11">
+        <f>ROUND(MAX(0,F4-G6*F5/1000-G8*F7/1000-G10*F9/1000),2)</f>
+        <v/>
+      </c>
+      <c r="G11" s="12" t="n"/>
+      <c r="J11" s="10" t="inlineStr">
+        <is>
+          <t>Required nmol needed</t>
+        </is>
+      </c>
+      <c r="K11" s="11">
+        <f>ROUND(MAX(0,K4-L6*K5/1000-L8*K7/1000-L10*K9/1000),2)</f>
+        <v/>
+      </c>
+      <c r="L11" s="12" t="n"/>
+    </row>
+    <row r="12">
+      <c r="E12" s="15" t="n"/>
+      <c r="F12" s="16" t="n"/>
+      <c r="G12" s="17" t="n"/>
+      <c r="J12" s="15" t="n"/>
+      <c r="K12" s="16" t="n"/>
+      <c r="L12" s="17" t="n"/>
+    </row>
+    <row r="13">
+      <c r="E13" s="18" t="inlineStr">
+        <is>
+          <t>Reagent</t>
+        </is>
+      </c>
+      <c r="F13" s="19" t="inlineStr">
+        <is>
+          <t>Final Conc.</t>
+        </is>
+      </c>
+      <c r="G13" s="20" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+      <c r="J13" s="18" t="inlineStr">
+        <is>
+          <t>Reagent</t>
+        </is>
+      </c>
+      <c r="K13" s="19" t="inlineStr">
+        <is>
+          <t>Final Conc.</t>
+        </is>
+      </c>
+      <c r="L13" s="20" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" s="21" t="inlineStr">
+        <is>
+          <t>hUba1 (uM)</t>
+        </is>
+      </c>
+      <c r="F14" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9">
+        <f>IF(C3&gt;0,(F14*2*F3)/C3,0)</f>
+        <v/>
+      </c>
+      <c r="J14" s="21" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="K14" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="9">
+        <f>IF(C4&gt;0,(K14*K3)/C4,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" s="21" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="F15" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9">
+        <f>IF(C4&gt;0,(F15*F3)/C4,0)</f>
+        <v/>
+      </c>
+      <c r="J15" s="21" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="K15" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="L15" s="9">
+        <f>IF(C5&gt;0,(K15*K3)/C5,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" s="21" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="F16" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="G16" s="9">
+        <f>IF(C5&gt;0,(F16*F3)/C5,0)</f>
+        <v/>
+      </c>
+      <c r="J16" s="18" t="inlineStr">
+        <is>
+          <t>HEPES buffer</t>
+        </is>
+      </c>
+      <c r="K16" s="23" t="inlineStr"/>
+      <c r="L16" s="14">
+        <f>K3-(L6+L8+L10+L14+L15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" s="18" t="inlineStr">
+        <is>
+          <t>HEPES buffer</t>
+        </is>
+      </c>
+      <c r="F17" s="23" t="inlineStr"/>
+      <c r="G17" s="14">
+        <f>F3-(G6+G8+G10+G14+G15+G16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20">
+      <c r="E20" s="6" t="inlineStr">
         <is>
           <t>Component</t>
         </is>
       </c>
-      <c r="E5" s="5">
-        <f>'Component Counts'!A2</f>
-        <v/>
-      </c>
-      <c r="F5" s="6" t="inlineStr">
+      <c r="F20" s="7">
+        <f>'Component Counts'!A3</f>
+        <v/>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
         <is>
           <t>Volume (uL)</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="D6" s="7" t="inlineStr">
+      <c r="J20" s="6" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="K20" s="7">
+        <f>'Component Counts'!A6</f>
+        <v/>
+      </c>
+      <c r="L20" s="5" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" s="10" t="inlineStr">
         <is>
           <t>Component Volume (uL)</t>
         </is>
       </c>
-      <c r="E6" s="8">
-        <f>'Component Counts'!D2</f>
-        <v/>
-      </c>
-      <c r="F6" s="9" t="n"/>
-    </row>
-    <row r="7">
-      <c r="D7" s="7" t="inlineStr">
+      <c r="F21" s="11">
+        <f>'Component Counts'!D3</f>
+        <v/>
+      </c>
+      <c r="G21" s="12" t="n"/>
+      <c r="J21" s="10" t="inlineStr">
+        <is>
+          <t>Component Volume (uL)</t>
+        </is>
+      </c>
+      <c r="K21" s="11">
+        <f>'Component Counts'!D6</f>
+        <v/>
+      </c>
+      <c r="L21" s="12" t="n"/>
+    </row>
+    <row r="22">
+      <c r="E22" s="10" t="inlineStr">
         <is>
           <t>Amount Needed (nmol)</t>
         </is>
       </c>
-      <c r="E7" s="8">
-        <f>'Component Counts'!F2</f>
-        <v/>
-      </c>
-      <c r="F7" s="9" t="n"/>
-    </row>
-    <row r="8">
-      <c r="D8" s="7" t="inlineStr">
+      <c r="F22" s="11">
+        <f>'Component Counts'!F3</f>
+        <v/>
+      </c>
+      <c r="G22" s="12" t="n"/>
+      <c r="J22" s="10" t="inlineStr">
+        <is>
+          <t>Amount Needed (nmol)</t>
+        </is>
+      </c>
+      <c r="K22" s="11">
+        <f>'Component Counts'!F6</f>
+        <v/>
+      </c>
+      <c r="L22" s="12" t="n"/>
+    </row>
+    <row r="23">
+      <c r="E23" s="10" t="inlineStr">
         <is>
           <t>Stock Conc. 1 (uM)</t>
         </is>
       </c>
-      <c r="E8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9" t="n"/>
-    </row>
-    <row r="9">
-      <c r="D9" s="7" t="inlineStr">
+      <c r="F23" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12" t="n"/>
+      <c r="J23" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 1 (uM)</t>
+        </is>
+      </c>
+      <c r="K23" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="12" t="n"/>
+    </row>
+    <row r="24">
+      <c r="E24" s="10" t="inlineStr">
         <is>
           <t>Stock Volume 1 (uL)</t>
         </is>
       </c>
-      <c r="E9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9">
-        <f>IF(AND(E8&gt;0,E7&gt;0),MIN(E9,ROUND(E7*1000/E8,2)),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="D10" s="7" t="inlineStr">
+      <c r="F24" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <f>IF(AND(F23&gt;0,F22&gt;0),MIN(F24,ROUND(F22*1000/F23,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J24" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 1 (uL)</t>
+        </is>
+      </c>
+      <c r="K24" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <f>IF(AND(K23&gt;0,K22&gt;0),MIN(K24,ROUND(K22*1000/K23,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" s="10" t="inlineStr">
         <is>
           <t>Stock Conc. 2 (uM)</t>
         </is>
       </c>
-      <c r="E10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9" t="n"/>
-    </row>
-    <row r="11">
-      <c r="D11" s="7" t="inlineStr">
+      <c r="F25" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12" t="n"/>
+      <c r="J25" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 2 (uM)</t>
+        </is>
+      </c>
+      <c r="K25" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="12" t="n"/>
+    </row>
+    <row r="26">
+      <c r="E26" s="10" t="inlineStr">
         <is>
           <t>Stock Volume 2 (uL)</t>
         </is>
       </c>
-      <c r="E11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="9">
-        <f>IF(AND(E10&gt;0,MAX(0,E7-F9*E8/1000)&gt;0),MIN(E11,ROUND(MAX(0,E7-F9*E8/1000)*1000/E10,2)),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="D12" s="7" t="inlineStr">
+      <c r="F26" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <f>IF(AND(F25&gt;0,MAX(0,F22-G24*F23/1000)&gt;0),MIN(F26,ROUND(MAX(0,F22-G24*F23/1000)*1000/F25,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J26" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 2 (uL)</t>
+        </is>
+      </c>
+      <c r="K26" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <f>IF(AND(K25&gt;0,MAX(0,K22-L24*K23/1000)&gt;0),MIN(K26,ROUND(MAX(0,K22-L24*K23/1000)*1000/K25,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" s="10" t="inlineStr">
         <is>
           <t>Stock Conc. 3 (uM)</t>
         </is>
       </c>
-      <c r="E12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9" t="n"/>
-    </row>
-    <row r="13">
-      <c r="D13" s="7" t="inlineStr">
+      <c r="F27" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="12" t="n"/>
+      <c r="J27" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 3 (uM)</t>
+        </is>
+      </c>
+      <c r="K27" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="12" t="n"/>
+    </row>
+    <row r="28">
+      <c r="E28" s="10" t="inlineStr">
         <is>
           <t>Stock Volume 3 (uL)</t>
         </is>
       </c>
-      <c r="E13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9">
-        <f>IF(AND(E12&gt;0,MAX(0,E7-F9*E8/1000-F11*E10/1000)&gt;0),MIN(G13,ROUND(MAX(0,E7-F9*E8/1000-F11*E10/1000)*1000/E12,2)),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14">
-      <c r="D14" s="7" t="inlineStr">
+      <c r="F28" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="12">
+        <f>IF(AND(F27&gt;0,MAX(0,F22-G24*F23/1000-G26*F25/1000)&gt;0),MIN(H28,ROUND(MAX(0,F22-G24*F23/1000-G26*F25/1000)*1000/F27,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J28" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 3 (uL)</t>
+        </is>
+      </c>
+      <c r="K28" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
+        <f>IF(AND(K27&gt;0,MAX(0,K22-L24*K23/1000-L26*K25/1000)&gt;0),MIN(M28,ROUND(MAX(0,K22-L24*K23/1000-L26*K25/1000)*1000/K27,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" s="10" t="inlineStr">
         <is>
           <t>Required nmol needed</t>
         </is>
       </c>
-      <c r="E14" s="8">
-        <f>ROUND(MAX(0,E7-F9*E8/1000-F11*E10/1000-F13*E12/1000),2)</f>
-        <v/>
-      </c>
-      <c r="F14" s="9" t="n"/>
-    </row>
-    <row r="15">
-      <c r="D15" s="10" t="n"/>
-      <c r="F15" s="9" t="n"/>
-    </row>
-    <row r="16">
-      <c r="D16" s="11" t="inlineStr">
+      <c r="F29" s="11">
+        <f>ROUND(MAX(0,F22-G24*F23/1000-G26*F25/1000-G28*F27/1000),2)</f>
+        <v/>
+      </c>
+      <c r="G29" s="12" t="n"/>
+      <c r="J29" s="10" t="inlineStr">
+        <is>
+          <t>Required nmol needed</t>
+        </is>
+      </c>
+      <c r="K29" s="11">
+        <f>ROUND(MAX(0,K22-L24*K23/1000-L26*K25/1000-L28*K27/1000),2)</f>
+        <v/>
+      </c>
+      <c r="L29" s="12" t="n"/>
+    </row>
+    <row r="30">
+      <c r="E30" s="15" t="n"/>
+      <c r="F30" s="16" t="n"/>
+      <c r="G30" s="17" t="n"/>
+      <c r="J30" s="15" t="n"/>
+      <c r="K30" s="16" t="n"/>
+      <c r="L30" s="17" t="n"/>
+    </row>
+    <row r="31">
+      <c r="E31" s="18" t="inlineStr">
         <is>
           <t>Reagent</t>
         </is>
       </c>
-      <c r="E16" s="12" t="inlineStr">
+      <c r="F31" s="19" t="inlineStr">
         <is>
           <t>Final Conc.</t>
         </is>
       </c>
-      <c r="F16" s="13" t="inlineStr">
+      <c r="G31" s="20" t="inlineStr">
         <is>
           <t>Volume (uL)</t>
         </is>
       </c>
-    </row>
-    <row r="17">
-      <c r="D17" s="11" t="inlineStr">
+      <c r="J31" s="18" t="inlineStr">
+        <is>
+          <t>Reagent</t>
+        </is>
+      </c>
+      <c r="K31" s="19" t="inlineStr">
+        <is>
+          <t>Final Conc.</t>
+        </is>
+      </c>
+      <c r="L31" s="20" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" s="21" t="inlineStr">
         <is>
           <t>hUba1 (uM)</t>
         </is>
       </c>
-      <c r="E17" s="12" t="n">
+      <c r="F32" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="13" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="D18" s="11" t="inlineStr">
+      <c r="G32" s="9">
+        <f>IF(C3&gt;0,(F32*2*F21)/C3,0)</f>
+        <v/>
+      </c>
+      <c r="J32" s="21" t="inlineStr">
         <is>
           <t>TCEP (mM)</t>
         </is>
       </c>
-      <c r="E18" s="12" t="n">
+      <c r="K32" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="13" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="D19" s="14" t="inlineStr">
+      <c r="L32" s="9">
+        <f>IF(C4&gt;0,(K32*K21)/C4,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" s="21" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="F33" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="9">
+        <f>IF(C4&gt;0,(F33*F21)/C4,0)</f>
+        <v/>
+      </c>
+      <c r="J33" s="21" t="inlineStr">
         <is>
           <t>ATP/Mg2+ (mM)</t>
         </is>
       </c>
-      <c r="E19" s="15" t="n">
+      <c r="K33" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="F19" s="16" t="inlineStr"/>
-    </row>
+      <c r="L33" s="9">
+        <f>IF(C5&gt;0,(K33*K21)/C5,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" s="21" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="F34" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="G34" s="9">
+        <f>IF(C5&gt;0,(F34*F21)/C5,0)</f>
+        <v/>
+      </c>
+      <c r="J34" s="18" t="inlineStr">
+        <is>
+          <t>HEPES buffer</t>
+        </is>
+      </c>
+      <c r="K34" s="23" t="inlineStr"/>
+      <c r="L34" s="14">
+        <f>K21-(L24+L26+L28+L32+L33)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" s="18" t="inlineStr">
+        <is>
+          <t>HEPES buffer</t>
+        </is>
+      </c>
+      <c r="F35" s="23" t="inlineStr"/>
+      <c r="G35" s="14">
+        <f>F21-(G24+G26+G28+G32+G33+G34)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38">
+      <c r="E38" s="6" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="F38" s="7">
+        <f>'Component Counts'!A4</f>
+        <v/>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+      <c r="J38" s="6" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="K38" s="7">
+        <f>'Component Counts'!A7</f>
+        <v/>
+      </c>
+      <c r="L38" s="5" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" s="10" t="inlineStr">
+        <is>
+          <t>Component Volume (uL)</t>
+        </is>
+      </c>
+      <c r="F39" s="11">
+        <f>'Component Counts'!D4</f>
+        <v/>
+      </c>
+      <c r="G39" s="12" t="n"/>
+      <c r="J39" s="10" t="inlineStr">
+        <is>
+          <t>Component Volume (uL)</t>
+        </is>
+      </c>
+      <c r="K39" s="11">
+        <f>'Component Counts'!D7</f>
+        <v/>
+      </c>
+      <c r="L39" s="12" t="n"/>
+    </row>
+    <row r="40">
+      <c r="E40" s="10" t="inlineStr">
+        <is>
+          <t>Amount Needed (nmol)</t>
+        </is>
+      </c>
+      <c r="F40" s="11">
+        <f>'Component Counts'!F4</f>
+        <v/>
+      </c>
+      <c r="G40" s="12" t="n"/>
+      <c r="J40" s="10" t="inlineStr">
+        <is>
+          <t>Amount Needed (nmol)</t>
+        </is>
+      </c>
+      <c r="K40" s="11">
+        <f>'Component Counts'!F7</f>
+        <v/>
+      </c>
+      <c r="L40" s="12" t="n"/>
+    </row>
+    <row r="41">
+      <c r="E41" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 1 (uM)</t>
+        </is>
+      </c>
+      <c r="F41" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="12" t="n"/>
+      <c r="J41" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 1 (uM)</t>
+        </is>
+      </c>
+      <c r="K41" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="12" t="n"/>
+    </row>
+    <row r="42">
+      <c r="E42" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 1 (uL)</t>
+        </is>
+      </c>
+      <c r="F42" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="12">
+        <f>IF(AND(F41&gt;0,F40&gt;0),MIN(F42,ROUND(F40*1000/F41,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J42" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 1 (uL)</t>
+        </is>
+      </c>
+      <c r="K42" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="12">
+        <f>IF(AND(K41&gt;0,K40&gt;0),MIN(K42,ROUND(K40*1000/K41,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 2 (uM)</t>
+        </is>
+      </c>
+      <c r="F43" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="12" t="n"/>
+      <c r="J43" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 2 (uM)</t>
+        </is>
+      </c>
+      <c r="K43" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="12" t="n"/>
+    </row>
+    <row r="44">
+      <c r="E44" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 2 (uL)</t>
+        </is>
+      </c>
+      <c r="F44" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="12">
+        <f>IF(AND(F43&gt;0,MAX(0,F40-G42*F41/1000)&gt;0),MIN(F44,ROUND(MAX(0,F40-G42*F41/1000)*1000/F43,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J44" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 2 (uL)</t>
+        </is>
+      </c>
+      <c r="K44" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="12">
+        <f>IF(AND(K43&gt;0,MAX(0,K40-L42*K41/1000)&gt;0),MIN(K44,ROUND(MAX(0,K40-L42*K41/1000)*1000/K43,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 3 (uM)</t>
+        </is>
+      </c>
+      <c r="F45" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="12" t="n"/>
+      <c r="J45" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 3 (uM)</t>
+        </is>
+      </c>
+      <c r="K45" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="12" t="n"/>
+    </row>
+    <row r="46">
+      <c r="E46" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 3 (uL)</t>
+        </is>
+      </c>
+      <c r="F46" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="12">
+        <f>IF(AND(F45&gt;0,MAX(0,F40-G42*F41/1000-G44*F43/1000)&gt;0),MIN(H46,ROUND(MAX(0,F40-G42*F41/1000-G44*F43/1000)*1000/F45,2)),0)</f>
+        <v/>
+      </c>
+      <c r="J46" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 3 (uL)</t>
+        </is>
+      </c>
+      <c r="K46" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="12">
+        <f>IF(AND(K45&gt;0,MAX(0,K40-L42*K41/1000-L44*K43/1000)&gt;0),MIN(M46,ROUND(MAX(0,K40-L42*K41/1000-L44*K43/1000)*1000/K45,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" s="10" t="inlineStr">
+        <is>
+          <t>Required nmol needed</t>
+        </is>
+      </c>
+      <c r="F47" s="11">
+        <f>ROUND(MAX(0,F40-G42*F41/1000-G44*F43/1000-G46*F45/1000),2)</f>
+        <v/>
+      </c>
+      <c r="G47" s="12" t="n"/>
+      <c r="J47" s="10" t="inlineStr">
+        <is>
+          <t>Required nmol needed</t>
+        </is>
+      </c>
+      <c r="K47" s="11">
+        <f>ROUND(MAX(0,K40-L42*K41/1000-L44*K43/1000-L46*K45/1000),2)</f>
+        <v/>
+      </c>
+      <c r="L47" s="12" t="n"/>
+    </row>
+    <row r="48">
+      <c r="E48" s="15" t="n"/>
+      <c r="F48" s="16" t="n"/>
+      <c r="G48" s="17" t="n"/>
+      <c r="J48" s="15" t="n"/>
+      <c r="K48" s="16" t="n"/>
+      <c r="L48" s="17" t="n"/>
+    </row>
+    <row r="49">
+      <c r="E49" s="18" t="inlineStr">
+        <is>
+          <t>Reagent</t>
+        </is>
+      </c>
+      <c r="F49" s="19" t="inlineStr">
+        <is>
+          <t>Final Conc.</t>
+        </is>
+      </c>
+      <c r="G49" s="20" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+      <c r="J49" s="18" t="inlineStr">
+        <is>
+          <t>Reagent</t>
+        </is>
+      </c>
+      <c r="K49" s="19" t="inlineStr">
+        <is>
+          <t>Final Conc.</t>
+        </is>
+      </c>
+      <c r="L49" s="20" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" s="21" t="inlineStr">
+        <is>
+          <t>hUba1 (uM)</t>
+        </is>
+      </c>
+      <c r="F50" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" s="9">
+        <f>IF(C3&gt;0,(F50*2*F39)/C3,0)</f>
+        <v/>
+      </c>
+      <c r="J50" s="21" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="K50" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L50" s="9">
+        <f>IF(C4&gt;0,(K50*K39)/C4,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" s="21" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="F51" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" s="9">
+        <f>IF(C4&gt;0,(F51*F39)/C4,0)</f>
+        <v/>
+      </c>
+      <c r="J51" s="21" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="K51" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="L51" s="9">
+        <f>IF(C5&gt;0,(K51*K39)/C5,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52">
+      <c r="E52" s="21" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="F52" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="G52" s="9">
+        <f>IF(C5&gt;0,(F52*F39)/C5,0)</f>
+        <v/>
+      </c>
+      <c r="J52" s="18" t="inlineStr">
+        <is>
+          <t>HEPES buffer</t>
+        </is>
+      </c>
+      <c r="K52" s="23" t="inlineStr"/>
+      <c r="L52" s="14">
+        <f>K39-(L42+L44+L46+L50+L51)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="E53" s="18" t="inlineStr">
+        <is>
+          <t>HEPES buffer</t>
+        </is>
+      </c>
+      <c r="F53" s="23" t="inlineStr"/>
+      <c r="G53" s="14">
+        <f>F39-(G42+G44+G46+G50+G51+G52)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56">
+      <c r="J56" s="6" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="K56" s="7">
+        <f>'Component Counts'!A8</f>
+        <v/>
+      </c>
+      <c r="L56" s="5" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>Component Volume (uL)</t>
+        </is>
+      </c>
+      <c r="K57" s="11">
+        <f>'Component Counts'!D8</f>
+        <v/>
+      </c>
+      <c r="L57" s="12" t="n"/>
+    </row>
+    <row r="58">
+      <c r="J58" s="10" t="inlineStr">
+        <is>
+          <t>Amount Needed (nmol)</t>
+        </is>
+      </c>
+      <c r="K58" s="11">
+        <f>'Component Counts'!F8</f>
+        <v/>
+      </c>
+      <c r="L58" s="12" t="n"/>
+    </row>
+    <row r="59">
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 1 (uM)</t>
+        </is>
+      </c>
+      <c r="K59" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" s="12" t="n"/>
+    </row>
+    <row r="60">
+      <c r="J60" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 1 (uL)</t>
+        </is>
+      </c>
+      <c r="K60" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" s="12">
+        <f>IF(AND(K59&gt;0,K58&gt;0),MIN(K60,ROUND(K58*1000/K59,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="J61" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 2 (uM)</t>
+        </is>
+      </c>
+      <c r="K61" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="12" t="n"/>
+    </row>
+    <row r="62">
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 2 (uL)</t>
+        </is>
+      </c>
+      <c r="K62" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" s="12">
+        <f>IF(AND(K61&gt;0,MAX(0,K58-L60*K59/1000)&gt;0),MIN(K62,ROUND(MAX(0,K58-L60*K59/1000)*1000/K61,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 3 (uM)</t>
+        </is>
+      </c>
+      <c r="K63" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" s="12" t="n"/>
+    </row>
+    <row r="64">
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 3 (uL)</t>
+        </is>
+      </c>
+      <c r="K64" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L64" s="12">
+        <f>IF(AND(K63&gt;0,MAX(0,K58-L60*K59/1000-L62*K61/1000)&gt;0),MIN(M64,ROUND(MAX(0,K58-L60*K59/1000-L62*K61/1000)*1000/K63,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>Required nmol needed</t>
+        </is>
+      </c>
+      <c r="K65" s="11">
+        <f>ROUND(MAX(0,K58-L60*K59/1000-L62*K61/1000-L64*K63/1000),2)</f>
+        <v/>
+      </c>
+      <c r="L65" s="12" t="n"/>
+    </row>
+    <row r="66">
+      <c r="J66" s="15" t="n"/>
+      <c r="K66" s="16" t="n"/>
+      <c r="L66" s="17" t="n"/>
+    </row>
+    <row r="67">
+      <c r="J67" s="18" t="inlineStr">
+        <is>
+          <t>Reagent</t>
+        </is>
+      </c>
+      <c r="K67" s="19" t="inlineStr">
+        <is>
+          <t>Final Conc.</t>
+        </is>
+      </c>
+      <c r="L67" s="20" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="J68" s="21" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="K68" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L68" s="9">
+        <f>IF(C4&gt;0,(K68*K57)/C4,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="J69" s="21" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="K69" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="L69" s="9">
+        <f>IF(C5&gt;0,(K69*K57)/C5,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70">
+      <c r="J70" s="18" t="inlineStr">
+        <is>
+          <t>HEPES buffer</t>
+        </is>
+      </c>
+      <c r="K70" s="23" t="inlineStr"/>
+      <c r="L70" s="14">
+        <f>K57-(L60+L62+L64+L68+L69)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71"/>
+    <row r="73"/>
+    <row r="74">
+      <c r="J74" s="6" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="K74" s="7">
+        <f>'Component Counts'!A9</f>
+        <v/>
+      </c>
+      <c r="L74" s="5" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>Component Volume (uL)</t>
+        </is>
+      </c>
+      <c r="K75" s="11">
+        <f>'Component Counts'!D9</f>
+        <v/>
+      </c>
+      <c r="L75" s="12" t="n"/>
+    </row>
+    <row r="76">
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>Amount Needed (nmol)</t>
+        </is>
+      </c>
+      <c r="K76" s="11">
+        <f>'Component Counts'!F9</f>
+        <v/>
+      </c>
+      <c r="L76" s="12" t="n"/>
+    </row>
+    <row r="77">
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 1 (uM)</t>
+        </is>
+      </c>
+      <c r="K77" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" s="12" t="n"/>
+    </row>
+    <row r="78">
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 1 (uL)</t>
+        </is>
+      </c>
+      <c r="K78" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" s="12">
+        <f>IF(AND(K77&gt;0,K76&gt;0),MIN(K78,ROUND(K76*1000/K77,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 2 (uM)</t>
+        </is>
+      </c>
+      <c r="K79" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" s="12" t="n"/>
+    </row>
+    <row r="80">
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 2 (uL)</t>
+        </is>
+      </c>
+      <c r="K80" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" s="12">
+        <f>IF(AND(K79&gt;0,MAX(0,K76-L78*K77/1000)&gt;0),MIN(K80,ROUND(MAX(0,K76-L78*K77/1000)*1000/K79,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81">
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>Stock Conc. 3 (uM)</t>
+        </is>
+      </c>
+      <c r="K81" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L81" s="12" t="n"/>
+    </row>
+    <row r="82">
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>Stock Volume 3 (uL)</t>
+        </is>
+      </c>
+      <c r="K82" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L82" s="12">
+        <f>IF(AND(K81&gt;0,MAX(0,K76-L78*K77/1000-L80*K79/1000)&gt;0),MIN(M82,ROUND(MAX(0,K76-L78*K77/1000-L80*K79/1000)*1000/K81,2)),0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83">
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>Required nmol needed</t>
+        </is>
+      </c>
+      <c r="K83" s="11">
+        <f>ROUND(MAX(0,K76-L78*K77/1000-L80*K79/1000-L82*K81/1000),2)</f>
+        <v/>
+      </c>
+      <c r="L83" s="12" t="n"/>
+    </row>
+    <row r="84">
+      <c r="J84" s="15" t="n"/>
+      <c r="K84" s="16" t="n"/>
+      <c r="L84" s="17" t="n"/>
+    </row>
+    <row r="85">
+      <c r="J85" s="18" t="inlineStr">
+        <is>
+          <t>Reagent</t>
+        </is>
+      </c>
+      <c r="K85" s="19" t="inlineStr">
+        <is>
+          <t>Final Conc.</t>
+        </is>
+      </c>
+      <c r="L85" s="20" t="inlineStr">
+        <is>
+          <t>Volume (uL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="J86" s="21" t="inlineStr">
+        <is>
+          <t>TCEP (mM)</t>
+        </is>
+      </c>
+      <c r="K86" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L86" s="9">
+        <f>IF(C4&gt;0,(K86*K75)/C4,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87">
+      <c r="J87" s="21" t="inlineStr">
+        <is>
+          <t>ATP/Mg2+ (mM)</t>
+        </is>
+      </c>
+      <c r="K87" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="L87" s="9">
+        <f>IF(C5&gt;0,(K87*K75)/C5,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88">
+      <c r="J88" s="18" t="inlineStr">
+        <is>
+          <t>HEPES buffer</t>
+        </is>
+      </c>
+      <c r="K88" s="23" t="inlineStr"/>
+      <c r="L88" s="14">
+        <f>K75-(L78+L80+L82+L86+L87)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Round Mass (mg) in Total hUba1 Needs box to 3 decimals in Excel output
- Updated the formula for the "Mass (mg)" cell in the Total hUba1 Needs box on the "Base Reagent Prep" worksheet to use =ROUND(C9*C10/1E6, 3).
- Ensures the value is always rounded to three decimal points for clarity and consistency.
</commit_message>
<xml_diff>
--- a/mixture_and_component_counts.xlsx
+++ b/mixture_and_component_counts.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekummelstedt/le_code_base/ubiquitinformatics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00D0A1C-BE4B-FA4A-A47C-37BDEBED3F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D77CFB-4E5A-D041-AE54-3BE080322C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mixture Counts" sheetId="1" r:id="rId1"/>
-    <sheet name="Component Counts" sheetId="2" r:id="rId2"/>
+    <sheet name="Mixed Reagents Counts" sheetId="1" r:id="rId1"/>
+    <sheet name="Base Reagent Counts" sheetId="2" r:id="rId2"/>
     <sheet name="Base Reagent Prep" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="56">
   <si>
     <t>Donor + Enzyme Mix</t>
   </si>
@@ -128,10 +128,10 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>Component Volume (uL)
+    <t>Base Reagent</t>
+  </si>
+  <si>
+    <t>Total Volume (uL)
 (Count * Reaction Volume (uL) * 1.1 / 2)</t>
   </si>
   <si>
@@ -143,11 +143,11 @@
 * Final Concentration (uM) * 1.1 / 1000)</t>
   </si>
   <si>
-    <t>Mass (Da)</t>
+    <t>MW (Da)</t>
   </si>
   <si>
     <t>Mass Required (mg)
-(Mass (Da) * Amount Needed (nmol) / 1000)</t>
+(MW (Da) * Amount Needed (nmol) / 1000)</t>
   </si>
   <si>
     <t>Stock Conc.</t>
@@ -159,7 +159,7 @@
     <t>hUba1 (uM)</t>
   </si>
   <si>
-    <t>Component Volume (uL)</t>
+    <t>Total Volume (uL)</t>
   </si>
   <si>
     <t>TCEP (mM)</t>
@@ -186,16 +186,16 @@
     <t>Stock Volume 2 (uL)</t>
   </si>
   <si>
-    <t>pmol</t>
+    <t>nmol</t>
   </si>
   <si>
     <t>Stock Conc. 3 (uM)</t>
   </si>
   <si>
+    <t>Stock Volume 3 (uL)</t>
+  </si>
+  <si>
     <t>Mass (mg)</t>
-  </si>
-  <si>
-    <t>Stock Volume 3 (uL)</t>
   </si>
   <si>
     <t>Required nmol needed</t>
@@ -420,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -455,20 +455,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -798,7 +789,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1038,32 +1031,32 @@
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>200</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
+        <v>220.00000000000003</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
+        <v>110.00000000000001</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>110.00000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1074,28 +1067,28 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>200</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>1320</v>
+        <v>660</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="1"/>
-        <v>660</v>
+        <v>330</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="2"/>
-        <v>660</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1138,28 +1131,28 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>200</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>880.00000000000011</v>
+        <v>220.00000000000003</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>440.00000000000006</v>
+        <v>110.00000000000001</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="2"/>
-        <v>440.00000000000006</v>
+        <v>110.00000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1202,28 +1195,28 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>200</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>1760.0000000000002</v>
+        <v>2420</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>880.00000000000011</v>
+        <v>1210</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="2"/>
-        <v>880.00000000000011</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1231,7 +1224,7 @@
         <v>29</v>
       </c>
       <c r="C14">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1246,7 @@
     <col min="4" max="4" width="42" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1308,8 +1301,8 @@
         <v>33800</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H9" si="2">IF(AND(ISNUMBER(G2),ISNUMBER(F2)),ROUND(G2*F2/1000000,2),)</f>
-        <v>1.78</v>
+        <f t="shared" ref="H2:H9" si="2">IF(AND(ISNUMBER(G2),ISNUMBER(F2)),ROUND(G2*F2/1000000,3),)</f>
+        <v>1.7849999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1338,7 +1331,7 @@
       </c>
       <c r="H3">
         <f t="shared" si="2"/>
-        <v>1.0900000000000001</v>
+        <v>1.093</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1346,28 +1339,28 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>200</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>770.00000000000011</v>
+        <v>550</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>30.800000000000004</v>
+        <v>22</v>
       </c>
       <c r="G4">
         <v>22400</v>
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>0.69</v>
+        <v>0.49299999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1396,7 +1389,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>0.57999999999999996</v>
+        <v>0.58399999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1404,28 +1397,28 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>200</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>550</v>
+        <v>220.00000000000003</v>
       </c>
       <c r="E6">
         <v>20</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="G6">
         <v>8864</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>7.8E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1433,28 +1426,28 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>200</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>880.00000000000011</v>
+        <v>990.00000000000011</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>35.200000000000003</v>
+        <v>39.6</v>
       </c>
       <c r="G7">
         <v>8864</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>0.31</v>
+        <v>0.35099999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1462,28 +1455,28 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>200</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>550</v>
+        <v>220.00000000000003</v>
       </c>
       <c r="E8">
         <v>20</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="G8">
         <v>8733</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>0.19</v>
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1524,18 +1517,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="5" max="7" width="23" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="5" max="7" width="22" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="28" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="16" x14ac:dyDescent="0.2">
@@ -1547,7 +1538,7 @@
         <v>30</v>
       </c>
       <c r="F2" s="6" t="str">
-        <f>'Component Counts'!A2</f>
+        <f>'Base Reagent Counts'!A2</f>
         <v>Ubc13/Mms2</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1557,7 +1548,7 @@
         <v>30</v>
       </c>
       <c r="K2" s="6" t="str">
-        <f>'Component Counts'!A5</f>
+        <f>'Base Reagent Counts'!A5</f>
         <v>ubi_ubq_1_K48_ABOC_K63_ABOC</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -1575,7 +1566,7 @@
         <v>39</v>
       </c>
       <c r="F3" s="10">
-        <f>'Component Counts'!D2</f>
+        <f>'Base Reagent Counts'!D2</f>
         <v>1320</v>
       </c>
       <c r="G3" s="11"/>
@@ -1583,7 +1574,7 @@
         <v>39</v>
       </c>
       <c r="K3" s="10">
-        <f>'Component Counts'!D5</f>
+        <f>'Base Reagent Counts'!D5</f>
         <v>1650.0000000000002</v>
       </c>
       <c r="L3" s="11"/>
@@ -1599,7 +1590,7 @@
         <v>41</v>
       </c>
       <c r="F4" s="10">
-        <f>'Component Counts'!F2</f>
+        <f>'Base Reagent Counts'!F2</f>
         <v>52.800000000000004</v>
       </c>
       <c r="G4" s="11"/>
@@ -1607,7 +1598,7 @@
         <v>41</v>
       </c>
       <c r="K4" s="10">
-        <f>'Component Counts'!F5</f>
+        <f>'Base Reagent Counts'!F5</f>
         <v>66</v>
       </c>
       <c r="L4" s="11"/>
@@ -1657,10 +1648,10 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="14"/>
       <c r="E7" s="9" t="s">
         <v>46</v>
       </c>
@@ -1677,10 +1668,13 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="15">
+        <f>G14+G32+G50</f>
+        <v>572</v>
+      </c>
       <c r="E8" s="9" t="s">
         <v>47</v>
       </c>
@@ -1703,10 +1697,13 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="15">
+        <f>C3*C8/1000</f>
+        <v>5.72</v>
+      </c>
       <c r="E9" s="9" t="s">
         <v>49</v>
       </c>
@@ -1723,12 +1720,14 @@
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="2:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="15">
+        <v>116300</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="E10" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="F10" s="10">
         <v>0</v>
@@ -1738,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K10" s="10">
         <v>0</v>
@@ -1749,6 +1748,13 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="16">
+        <f>ROUND(C9*C10/1000000, 3)</f>
+        <v>0.66500000000000004</v>
+      </c>
       <c r="E11" s="9" t="s">
         <v>52</v>
       </c>
@@ -1767,48 +1773,48 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="22"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="24">
         <v>1</v>
       </c>
       <c r="G14" s="8">
         <f>IF(C3&gt;0,(F14*2*F3)/C3,0)</f>
         <v>264</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="27">
+      <c r="K14" s="24">
         <v>1</v>
       </c>
       <c r="L14" s="8">
@@ -1817,20 +1823,20 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="24">
         <v>1</v>
       </c>
       <c r="G15" s="8">
         <f>IF(C4&gt;0,(F15*F3)/C4,0)</f>
         <v>132</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K15" s="24">
         <v>10</v>
       </c>
       <c r="L15" s="8">
@@ -1839,30 +1845,30 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="24">
         <v>10</v>
       </c>
       <c r="G16" s="8">
         <f>IF(C5&gt;0,(F16*F3)/C5,0)</f>
         <v>132</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="K16" s="28"/>
+      <c r="K16" s="25"/>
       <c r="L16" s="13">
         <f>K3-(L6+L8+L10+L14+L15)</f>
         <v>1320.0000000000002</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="28"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="13">
         <f>F3-(G6+G8+G10+G14+G15+G16)</f>
         <v>792</v>
@@ -1873,7 +1879,7 @@
         <v>30</v>
       </c>
       <c r="F20" s="6" t="str">
-        <f>'Component Counts'!A3</f>
+        <f>'Base Reagent Counts'!A3</f>
         <v>gp78/Ube2g2</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -1883,7 +1889,7 @@
         <v>30</v>
       </c>
       <c r="K20" s="6" t="str">
-        <f>'Component Counts'!A6</f>
+        <f>'Base Reagent Counts'!A6</f>
         <v>ubi_ubq_1_K48_SMAC_K63_ABOC</v>
       </c>
       <c r="L20" s="4" t="s">
@@ -1895,7 +1901,7 @@
         <v>39</v>
       </c>
       <c r="F21" s="10">
-        <f>'Component Counts'!D3</f>
+        <f>'Base Reagent Counts'!D3</f>
         <v>990.00000000000011</v>
       </c>
       <c r="G21" s="11"/>
@@ -1903,8 +1909,8 @@
         <v>39</v>
       </c>
       <c r="K21" s="10">
-        <f>'Component Counts'!D6</f>
-        <v>550</v>
+        <f>'Base Reagent Counts'!D6</f>
+        <v>220.00000000000003</v>
       </c>
       <c r="L21" s="11"/>
     </row>
@@ -1913,7 +1919,7 @@
         <v>41</v>
       </c>
       <c r="F22" s="10">
-        <f>'Component Counts'!F3</f>
+        <f>'Base Reagent Counts'!F3</f>
         <v>39.6</v>
       </c>
       <c r="G22" s="11"/>
@@ -1921,8 +1927,8 @@
         <v>41</v>
       </c>
       <c r="K22" s="10">
-        <f>'Component Counts'!F6</f>
-        <v>22</v>
+        <f>'Base Reagent Counts'!F6</f>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L22" s="11"/>
     </row>
@@ -2020,7 +2026,7 @@
     </row>
     <row r="28" spans="5:12" ht="16" x14ac:dyDescent="0.2">
       <c r="E28" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F28" s="10">
         <v>0</v>
@@ -2030,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K28" s="10">
         <v>0</v>
@@ -2054,107 +2060,107 @@
       </c>
       <c r="K29" s="10">
         <f>ROUND(MAX(0,K22-L24*K23/1000-L26*K25/1000-L28*K27/1000),2)</f>
-        <v>22</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L29" s="11"/>
     </row>
     <row r="30" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="22"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="19"/>
     </row>
     <row r="31" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="25" t="s">
+      <c r="G31" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J31" s="23" t="s">
+      <c r="J31" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K31" s="24" t="s">
+      <c r="K31" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L31" s="25" t="s">
+      <c r="L31" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="24">
         <v>1</v>
       </c>
       <c r="G32" s="8">
         <f>IF(C3&gt;0,(F32*2*F21)/C3,0)</f>
         <v>198.00000000000003</v>
       </c>
-      <c r="J32" s="26" t="s">
+      <c r="J32" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="K32" s="27">
+      <c r="K32" s="24">
         <v>1</v>
       </c>
       <c r="L32" s="8">
         <f>IF(C4&gt;0,(K32*K21)/C4,0)</f>
-        <v>55</v>
+        <v>22.000000000000004</v>
       </c>
     </row>
     <row r="33" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="24">
         <v>1</v>
       </c>
       <c r="G33" s="8">
         <f>IF(C4&gt;0,(F33*F21)/C4,0)</f>
         <v>99.000000000000014</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="J33" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="K33" s="27">
+      <c r="K33" s="24">
         <v>10</v>
       </c>
       <c r="L33" s="8">
         <f>IF(C5&gt;0,(K33*K21)/C5,0)</f>
-        <v>55</v>
+        <v>22.000000000000004</v>
       </c>
     </row>
     <row r="34" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="24">
         <v>10</v>
       </c>
       <c r="G34" s="8">
         <f>IF(C5&gt;0,(F34*F21)/C5,0)</f>
         <v>99.000000000000014</v>
       </c>
-      <c r="J34" s="23" t="s">
+      <c r="J34" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="K34" s="28"/>
+      <c r="K34" s="25"/>
       <c r="L34" s="13">
         <f>K21-(L24+L26+L28+L32+L33)</f>
-        <v>440</v>
+        <v>176.00000000000003</v>
       </c>
     </row>
     <row r="35" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F35" s="28"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="13">
         <f>F21-(G24+G26+G28+G32+G33+G34)</f>
         <v>594</v>
@@ -2165,7 +2171,7 @@
         <v>30</v>
       </c>
       <c r="F38" s="6" t="str">
-        <f>'Component Counts'!A4</f>
+        <f>'Base Reagent Counts'!A4</f>
         <v>Ube2K</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -2175,7 +2181,7 @@
         <v>30</v>
       </c>
       <c r="K38" s="6" t="str">
-        <f>'Component Counts'!A7</f>
+        <f>'Base Reagent Counts'!A7</f>
         <v>ubi_ubq_1_K48_ABOC_K63_SMAC</v>
       </c>
       <c r="L38" s="4" t="s">
@@ -2187,16 +2193,16 @@
         <v>39</v>
       </c>
       <c r="F39" s="10">
-        <f>'Component Counts'!D4</f>
-        <v>770.00000000000011</v>
+        <f>'Base Reagent Counts'!D4</f>
+        <v>550</v>
       </c>
       <c r="G39" s="11"/>
       <c r="J39" s="9" t="s">
         <v>39</v>
       </c>
       <c r="K39" s="10">
-        <f>'Component Counts'!D7</f>
-        <v>880.00000000000011</v>
+        <f>'Base Reagent Counts'!D7</f>
+        <v>990.00000000000011</v>
       </c>
       <c r="L39" s="11"/>
     </row>
@@ -2205,16 +2211,16 @@
         <v>41</v>
       </c>
       <c r="F40" s="10">
-        <f>'Component Counts'!F4</f>
-        <v>30.800000000000004</v>
+        <f>'Base Reagent Counts'!F4</f>
+        <v>22</v>
       </c>
       <c r="G40" s="11"/>
       <c r="J40" s="9" t="s">
         <v>41</v>
       </c>
       <c r="K40" s="10">
-        <f>'Component Counts'!F7</f>
-        <v>35.200000000000003</v>
+        <f>'Base Reagent Counts'!F7</f>
+        <v>39.6</v>
       </c>
       <c r="L40" s="11"/>
     </row>
@@ -2312,7 +2318,7 @@
     </row>
     <row r="46" spans="5:12" ht="16" x14ac:dyDescent="0.2">
       <c r="E46" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F46" s="10">
         <v>0</v>
@@ -2322,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K46" s="10">
         <v>0</v>
@@ -2338,7 +2344,7 @@
       </c>
       <c r="F47" s="10">
         <f>ROUND(MAX(0,F40-G42*F41/1000-G44*F43/1000-G46*F45/1000),2)</f>
-        <v>30.8</v>
+        <v>22</v>
       </c>
       <c r="G47" s="11"/>
       <c r="J47" s="9" t="s">
@@ -2346,110 +2352,110 @@
       </c>
       <c r="K47" s="10">
         <f>ROUND(MAX(0,K40-L42*K41/1000-L44*K43/1000-L46*K45/1000),2)</f>
-        <v>35.200000000000003</v>
+        <v>39.6</v>
       </c>
       <c r="L47" s="11"/>
     </row>
     <row r="48" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E48" s="20"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="22"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="22"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="19"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="19"/>
     </row>
     <row r="49" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E49" s="23" t="s">
+      <c r="E49" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F49" s="24" t="s">
+      <c r="F49" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="G49" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J49" s="23" t="s">
+      <c r="J49" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K49" s="24" t="s">
+      <c r="K49" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L49" s="25" t="s">
+      <c r="L49" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="50" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E50" s="26" t="s">
+      <c r="E50" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F50" s="27">
+      <c r="F50" s="24">
         <v>1</v>
       </c>
       <c r="G50" s="8">
         <f>IF(C3&gt;0,(F50*2*F39)/C3,0)</f>
-        <v>154.00000000000003</v>
-      </c>
-      <c r="J50" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="J50" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="K50" s="27">
+      <c r="K50" s="24">
         <v>1</v>
       </c>
       <c r="L50" s="8">
         <f>IF(C4&gt;0,(K50*K39)/C4,0)</f>
-        <v>88.000000000000014</v>
+        <v>99.000000000000014</v>
       </c>
     </row>
     <row r="51" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E51" s="26" t="s">
+      <c r="E51" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F51" s="27">
+      <c r="F51" s="24">
         <v>1</v>
       </c>
       <c r="G51" s="8">
         <f>IF(C4&gt;0,(F51*F39)/C4,0)</f>
-        <v>77.000000000000014</v>
-      </c>
-      <c r="J51" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J51" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="K51" s="27">
+      <c r="K51" s="24">
         <v>10</v>
       </c>
       <c r="L51" s="8">
         <f>IF(C5&gt;0,(K51*K39)/C5,0)</f>
-        <v>88.000000000000014</v>
+        <v>99.000000000000014</v>
       </c>
     </row>
     <row r="52" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E52" s="26" t="s">
+      <c r="E52" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F52" s="27">
+      <c r="F52" s="24">
         <v>10</v>
       </c>
       <c r="G52" s="8">
         <f>IF(C5&gt;0,(F52*F39)/C5,0)</f>
-        <v>77.000000000000014</v>
-      </c>
-      <c r="J52" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="K52" s="28"/>
+      <c r="J52" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="K52" s="25"/>
       <c r="L52" s="13">
         <f>K39-(L42+L44+L46+L50+L51)</f>
-        <v>704.00000000000011</v>
+        <v>792.00000000000011</v>
       </c>
     </row>
     <row r="53" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E53" s="23" t="s">
+      <c r="E53" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F53" s="28"/>
+      <c r="F53" s="25"/>
       <c r="G53" s="13">
         <f>F39-(G42+G44+G46+G50+G51+G52)</f>
-        <v>462.00000000000006</v>
+        <v>330</v>
       </c>
     </row>
     <row r="56" spans="5:12" ht="16" x14ac:dyDescent="0.2">
@@ -2457,7 +2463,7 @@
         <v>30</v>
       </c>
       <c r="K56" s="6" t="str">
-        <f>'Component Counts'!A8</f>
+        <f>'Base Reagent Counts'!A8</f>
         <v>ubi_ubq_1_K48_SMAC</v>
       </c>
       <c r="L56" s="4" t="s">
@@ -2469,8 +2475,8 @@
         <v>39</v>
       </c>
       <c r="K57" s="10">
-        <f>'Component Counts'!D8</f>
-        <v>550</v>
+        <f>'Base Reagent Counts'!D8</f>
+        <v>220.00000000000003</v>
       </c>
       <c r="L57" s="11"/>
     </row>
@@ -2479,8 +2485,8 @@
         <v>41</v>
       </c>
       <c r="K58" s="10">
-        <f>'Component Counts'!F8</f>
-        <v>22</v>
+        <f>'Base Reagent Counts'!F8</f>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L58" s="11"/>
     </row>
@@ -2537,7 +2543,7 @@
     </row>
     <row r="64" spans="5:12" ht="16" x14ac:dyDescent="0.2">
       <c r="J64" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K64" s="10">
         <v>0</v>
@@ -2553,58 +2559,58 @@
       </c>
       <c r="K65" s="10">
         <f>ROUND(MAX(0,K58-L60*K59/1000-L62*K61/1000-L64*K63/1000),2)</f>
-        <v>22</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L65" s="11"/>
     </row>
     <row r="66" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J66" s="20"/>
-      <c r="K66" s="21"/>
-      <c r="L66" s="22"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="19"/>
     </row>
     <row r="67" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J67" s="23" t="s">
+      <c r="J67" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K67" s="24" t="s">
+      <c r="K67" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L67" s="25" t="s">
+      <c r="L67" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="68" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J68" s="26" t="s">
+      <c r="J68" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="K68" s="27">
+      <c r="K68" s="24">
         <v>1</v>
       </c>
       <c r="L68" s="8">
         <f>IF(C4&gt;0,(K68*K57)/C4,0)</f>
-        <v>55</v>
+        <v>22.000000000000004</v>
       </c>
     </row>
     <row r="69" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J69" s="26" t="s">
+      <c r="J69" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="K69" s="27">
+      <c r="K69" s="24">
         <v>10</v>
       </c>
       <c r="L69" s="8">
         <f>IF(C5&gt;0,(K69*K57)/C5,0)</f>
+        <v>22.000000000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J70" s="20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="70" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J70" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="K70" s="28"/>
+      <c r="K70" s="25"/>
       <c r="L70" s="13">
         <f>K57-(L60+L62+L64+L68+L69)</f>
-        <v>440</v>
+        <v>176.00000000000003</v>
       </c>
     </row>
     <row r="74" spans="10:12" ht="16" x14ac:dyDescent="0.2">
@@ -2612,7 +2618,7 @@
         <v>30</v>
       </c>
       <c r="K74" s="6" t="str">
-        <f>'Component Counts'!A9</f>
+        <f>'Base Reagent Counts'!A9</f>
         <v>ubi_ubq_1_K63_SMAC</v>
       </c>
       <c r="L74" s="4" t="s">
@@ -2624,7 +2630,7 @@
         <v>39</v>
       </c>
       <c r="K75" s="10">
-        <f>'Component Counts'!D9</f>
+        <f>'Base Reagent Counts'!D9</f>
         <v>0</v>
       </c>
       <c r="L75" s="11"/>
@@ -2634,7 +2640,7 @@
         <v>41</v>
       </c>
       <c r="K76" s="10">
-        <f>'Component Counts'!F9</f>
+        <f>'Base Reagent Counts'!F9</f>
         <v>0</v>
       </c>
       <c r="L76" s="11"/>
@@ -2692,7 +2698,7 @@
     </row>
     <row r="82" spans="10:12" ht="16" x14ac:dyDescent="0.2">
       <c r="J82" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K82" s="10">
         <v>0</v>
@@ -2713,26 +2719,26 @@
       <c r="L83" s="11"/>
     </row>
     <row r="84" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J84" s="20"/>
-      <c r="K84" s="21"/>
-      <c r="L84" s="22"/>
+      <c r="J84" s="17"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="19"/>
     </row>
     <row r="85" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J85" s="23" t="s">
+      <c r="J85" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K85" s="24" t="s">
+      <c r="K85" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L85" s="25" t="s">
+      <c r="L85" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="86" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J86" s="26" t="s">
+      <c r="J86" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="K86" s="27">
+      <c r="K86" s="24">
         <v>1</v>
       </c>
       <c r="L86" s="8">
@@ -2741,10 +2747,10 @@
       </c>
     </row>
     <row r="87" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J87" s="26" t="s">
+      <c r="J87" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="K87" s="27">
+      <c r="K87" s="24">
         <v>10</v>
       </c>
       <c r="L87" s="8">
@@ -2753,10 +2759,10 @@
       </c>
     </row>
     <row r="88" spans="10:12" x14ac:dyDescent="0.2">
-      <c r="J88" s="23" t="s">
+      <c r="J88" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="K88" s="28"/>
+      <c r="K88" s="25"/>
       <c r="L88" s="13">
         <f>K75-(L78+L80+L82+L86+L87)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Refactor Excel export: generate workbook in memory using BytesIO for FastAPI compatibility, remove disk writes, and add instructions for saving BytesIO to file for local viewing.
</commit_message>
<xml_diff>
--- a/mixture_and_component_counts.xlsx
+++ b/mixture_and_component_counts.xlsx
@@ -47,7 +47,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -60,6 +60,9 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
     </border>
     <border>
       <left/>
@@ -152,70 +155,70 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -586,536 +589,603 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="48" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
-    <col width="22" customWidth="1" min="4" max="4"/>
-    <col width="38" customWidth="1" min="5" max="5"/>
-    <col width="29" customWidth="1" min="6" max="6"/>
-    <col width="19" customWidth="1" min="7" max="7"/>
-    <col width="13" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="48" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="38" customWidth="1" min="6" max="6"/>
+    <col width="29" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="19" customWidth="1" min="9" max="9"/>
+    <col width="13" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1"/>
+    <row r="2">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Donor + Enzyme Mix</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Donor + Enzyme Id</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Reaction Volume (uL)</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Donor + Enzyme Volume (uL)
 (Count * Reaction Volume (uL) * 1.1)</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Donor</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Donor Id</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>Donor Volume (uL)</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>Enzyme</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>Enzyme Volume (uL)</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="3">
+      <c r="B3" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_SMAC', 'gp78/Ube2g2')</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
         <v>200</v>
       </c>
-      <c r="E2">
-        <f>C2*D2*1.1</f>
-        <v/>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="F3">
+        <f>E3*D3*1.1</f>
+        <v/>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_SMAC</t>
         </is>
       </c>
-      <c r="G2">
-        <f>(C2*D2*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 1</t>
+        </is>
+      </c>
+      <c r="I3">
+        <f>(D3*E3*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>gp78/Ube2g2</t>
         </is>
       </c>
-      <c r="I2">
-        <f>(C2*D2*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="K3">
+        <f>(D3*E3*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_SMAC_K63_ABOC', 'gp78/Ube2g2')</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C4" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>200</v>
       </c>
-      <c r="E3">
-        <f>C3*D3*1.1</f>
-        <v/>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="F4">
+        <f>E4*D4*1.1</f>
+        <v/>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_SMAC_K63_ABOC</t>
         </is>
       </c>
-      <c r="G3">
-        <f>(C3*D3*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H3" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 2</t>
+        </is>
+      </c>
+      <c r="I4">
+        <f>(D4*E4*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>gp78/Ube2g2</t>
         </is>
       </c>
-      <c r="I3">
-        <f>(C3*D3*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="K4">
+        <f>(D4*E4*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_ABOC_K63_SMAC', 'gp78/Ube2g2')</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="C5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D5" t="n">
         <v>8</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E5" t="n">
         <v>200</v>
       </c>
-      <c r="E4">
-        <f>C4*D4*1.1</f>
-        <v/>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="F5">
+        <f>E5*D5*1.1</f>
+        <v/>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_ABOC_K63_SMAC</t>
         </is>
       </c>
-      <c r="G4" s="3">
-        <f>(C4*D4*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H4" s="3" t="inlineStr">
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 4</t>
+        </is>
+      </c>
+      <c r="I5" s="3">
+        <f>(D5*E5*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
         <is>
           <t>gp78/Ube2g2</t>
         </is>
       </c>
-      <c r="I4" s="3">
-        <f>(C4*D4*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="K5" s="3">
+        <f>(D5*E5*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_ABOC_K63_ABOC', 'gp78/Ube2g2')</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="C6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E6" t="n">
         <v>200</v>
       </c>
-      <c r="E5">
-        <f>C5*D5*1.1</f>
-        <v/>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F6">
+        <f>E6*D6*1.1</f>
+        <v/>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_ABOC_K63_ABOC</t>
         </is>
       </c>
-      <c r="G5" s="3">
-        <f>(C5*D5*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H5" s="3" t="inlineStr">
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 5</t>
+        </is>
+      </c>
+      <c r="I6" s="3">
+        <f>(D6*E6*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
         <is>
           <t>gp78/Ube2g2</t>
         </is>
       </c>
-      <c r="I5" s="3">
-        <f>(C5*D5*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="K6" s="3">
+        <f>(D6*E6*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_SMAC', 'Ube2K')</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C7" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>200</v>
       </c>
-      <c r="E6">
-        <f>C6*D6*1.1</f>
-        <v/>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="F7">
+        <f>E7*D7*1.1</f>
+        <v/>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_SMAC</t>
         </is>
       </c>
-      <c r="G6">
-        <f>(C6*D6*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 1</t>
+        </is>
+      </c>
+      <c r="I7">
+        <f>(D7*E7*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>Ube2K</t>
         </is>
       </c>
-      <c r="I6">
-        <f>(C6*D6*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="K7">
+        <f>(D7*E7*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_SMAC_K63_ABOC', 'Ube2K')</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="C8" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E8" t="n">
         <v>200</v>
       </c>
-      <c r="E7">
-        <f>C7*D7*1.1</f>
-        <v/>
-      </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F8">
+        <f>E8*D8*1.1</f>
+        <v/>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_SMAC_K63_ABOC</t>
         </is>
       </c>
-      <c r="G7" s="3">
-        <f>(C7*D7*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H7" s="3" t="inlineStr">
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 2</t>
+        </is>
+      </c>
+      <c r="I8" s="3">
+        <f>(D8*E8*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
         <is>
           <t>Ube2K</t>
         </is>
       </c>
-      <c r="I7" s="3">
-        <f>(C7*D7*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="K8" s="3">
+        <f>(D8*E8*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_ABOC_K63_SMAC', 'Ube2K')</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="C9" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D9" t="n">
         <v>1</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E9" t="n">
         <v>200</v>
       </c>
-      <c r="E8">
-        <f>C8*D8*1.1</f>
-        <v/>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="F9">
+        <f>E9*D9*1.1</f>
+        <v/>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_ABOC_K63_SMAC</t>
         </is>
       </c>
-      <c r="G8" s="3">
-        <f>(C8*D8*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H8" s="3" t="inlineStr">
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 4</t>
+        </is>
+      </c>
+      <c r="I9" s="3">
+        <f>(D9*E9*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
         <is>
           <t>Ube2K</t>
         </is>
       </c>
-      <c r="I8" s="3">
-        <f>(C8*D8*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="K9" s="3">
+        <f>(D9*E9*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_ABOC_K63_ABOC', 'Ube2K')</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="C10" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D10" t="n">
         <v>3</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E10" t="n">
         <v>200</v>
       </c>
-      <c r="E9">
-        <f>C9*D9*1.1</f>
-        <v/>
-      </c>
-      <c r="F9" s="3" t="inlineStr">
+      <c r="F10">
+        <f>E10*D10*1.1</f>
+        <v/>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_ABOC_K63_ABOC</t>
         </is>
       </c>
-      <c r="G9" s="3">
-        <f>(C9*D9*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H9" s="3" t="inlineStr">
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 5</t>
+        </is>
+      </c>
+      <c r="I10" s="3">
+        <f>(D10*E10*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
         <is>
           <t>Ube2K</t>
         </is>
       </c>
-      <c r="I9" s="3">
-        <f>(C9*D9*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="K10" s="3">
+        <f>(D10*E10*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K63_SMAC', 'Ubc13/Mms2')</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C11" t="n">
         <v>9</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
         <v>200</v>
       </c>
-      <c r="E10">
-        <f>C10*D10*1.1</f>
-        <v/>
-      </c>
-      <c r="F10" t="inlineStr">
+      <c r="F11">
+        <f>E11*D11*1.1</f>
+        <v/>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K63_SMAC</t>
         </is>
       </c>
-      <c r="G10">
-        <f>(C10*D10*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 3</t>
+        </is>
+      </c>
+      <c r="I11">
+        <f>(D11*E11*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>Ubc13/Mms2</t>
         </is>
       </c>
-      <c r="I10">
-        <f>(C10*D10*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="K11">
+        <f>(D11*E11*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_SMAC_K63_ABOC', 'Ubc13/Mms2')</t>
         </is>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="C12" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D12" t="n">
         <v>1</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E12" t="n">
         <v>200</v>
       </c>
-      <c r="E11">
-        <f>C11*D11*1.1</f>
-        <v/>
-      </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="F12">
+        <f>E12*D12*1.1</f>
+        <v/>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_SMAC_K63_ABOC</t>
         </is>
       </c>
-      <c r="G11" s="3">
-        <f>(C11*D11*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H11" s="3" t="inlineStr">
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 2</t>
+        </is>
+      </c>
+      <c r="I12" s="3">
+        <f>(D12*E12*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
         <is>
           <t>Ubc13/Mms2</t>
         </is>
       </c>
-      <c r="I11" s="3">
-        <f>(C11*D11*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="K12" s="3">
+        <f>(D12*E12*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
         <is>
           <t>('ubi_ubq_1_K48_ABOC_K63_SMAC', 'Ubc13/Mms2')</t>
         </is>
-      </c>
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>200</v>
-      </c>
-      <c r="E12">
-        <f>C12*D12*1.1</f>
-        <v/>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>ubi_ubq_1_K48_ABOC_K63_SMAC</t>
-        </is>
-      </c>
-      <c r="G12">
-        <f>(C12*D12*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Ubc13/Mms2</t>
-        </is>
-      </c>
-      <c r="I12">
-        <f>(C12*D12*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>('ubi_ubq_1_K48_ABOC_K63_ABOC', 'Ubc13/Mms2')</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>12</v>
       </c>
       <c r="C13" t="n">
         <v>11</v>
       </c>
       <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
         <v>200</v>
       </c>
-      <c r="E13">
-        <f>C13*D13*1.1</f>
-        <v/>
-      </c>
-      <c r="F13" s="3" t="inlineStr">
+      <c r="F13">
+        <f>E13*D13*1.1</f>
+        <v/>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>ubi_ubq_1_K48_ABOC_K63_SMAC</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 4</t>
+        </is>
+      </c>
+      <c r="I13">
+        <f>(D13*E13*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Ubc13/Mms2</t>
+        </is>
+      </c>
+      <c r="K13">
+        <f>(D13*E13*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>('ubi_ubq_1_K48_ABOC_K63_ABOC', 'Ubc13/Mms2')</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="n">
+        <v>11</v>
+      </c>
+      <c r="E14" t="n">
+        <v>200</v>
+      </c>
+      <c r="F14">
+        <f>E14*D14*1.1</f>
+        <v/>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_ABOC_K63_ABOC</t>
         </is>
       </c>
-      <c r="G13" s="3">
-        <f>(C13*D13*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="H13" s="3" t="inlineStr">
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>Donor: Ubᴰ 5</t>
+        </is>
+      </c>
+      <c r="I14" s="3">
+        <f>(D14*E14*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
         <is>
           <t>Ubc13/Mms2</t>
         </is>
       </c>
-      <c r="I13" s="3">
-        <f>(C13*D13*1.1)/2</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="K14" s="3">
+        <f>(D14*E14*1.1)/2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="D15" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1130,315 +1200,350 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="29" customWidth="1" min="1" max="1"/>
-    <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="42" customWidth="1" min="4" max="4"/>
-    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="29" customWidth="1" min="2" max="2"/>
+    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="42" customWidth="1" min="6" max="6"/>
-    <col width="9" customWidth="1" min="7" max="7"/>
-    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="26" customWidth="1" min="7" max="7"/>
+    <col width="42" customWidth="1" min="8" max="8"/>
+    <col width="9" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1"/>
+    <row r="2">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Base Reagent</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Donor Id</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Reaction Volume (uL)</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Total Volume (uL)
 (Count * Reaction Volume (uL) * 1.1 / 2)</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>Final Concentration (uM)</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>Amount Needed (nmol)
 (Count * Reaction Volume (uL)
 * Final Concentration (uM) * 1.1 / 1000)</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>MW (Da)</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="J2" s="2" t="inlineStr">
         <is>
           <t>Mass Required (mg)
 (MW (Da) * Amount Needed (nmol) / 1000)</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="3">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Ubc13/Mms2</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C3" t="n">
         <v>12</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
         <v>200</v>
       </c>
-      <c r="D2">
-        <f>(B2*C2*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="E2" t="n">
+      <c r="F3">
+        <f>(C3*E3*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="G3" t="n">
         <v>20</v>
       </c>
-      <c r="F2">
-        <f>(B2*C2*E2*1.1/1000)</f>
-        <v/>
-      </c>
-      <c r="G2" t="n">
+      <c r="H3">
+        <f>(C3*E3*G3*1.1/1000)</f>
+        <v/>
+      </c>
+      <c r="I3" t="n">
         <v>33800</v>
       </c>
-      <c r="H2">
-        <f>IF(AND(ISNUMBER(G2),ISNUMBER(F2)),ROUND(G2*F2/1000000,3),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="J3">
+        <f>IF(AND(ISNUMBER(I3),ISNUMBER(H3)),ROUND(I3*H3/1000000,3),)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
         <is>
           <t>gp78/Ube2g2</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C4" t="n">
         <v>9</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
         <v>200</v>
       </c>
-      <c r="D3">
-        <f>(B3*C3*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="E3" t="n">
+      <c r="F4">
+        <f>(C4*E4*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="G4" t="n">
         <v>20</v>
       </c>
-      <c r="F3">
-        <f>(B3*C3*E3*1.1/1000)</f>
-        <v/>
-      </c>
-      <c r="G3" t="n">
+      <c r="H4">
+        <f>(C4*E4*G4*1.1/1000)</f>
+        <v/>
+      </c>
+      <c r="I4" t="n">
         <v>27600</v>
       </c>
-      <c r="H3">
-        <f>IF(AND(ISNUMBER(G3),ISNUMBER(F3)),ROUND(G3*F3/1000000,3),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="J4">
+        <f>IF(AND(ISNUMBER(I4),ISNUMBER(H4)),ROUND(I4*H4/1000000,3),)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Ube2K</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C5" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
         <v>200</v>
       </c>
-      <c r="D4">
-        <f>(B4*C4*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="E4" t="n">
+      <c r="F5">
+        <f>(C5*E5*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="G5" t="n">
         <v>20</v>
       </c>
-      <c r="F4">
-        <f>(B4*C4*E4*1.1/1000)</f>
-        <v/>
-      </c>
-      <c r="G4" t="n">
+      <c r="H5">
+        <f>(C5*E5*G5*1.1/1000)</f>
+        <v/>
+      </c>
+      <c r="I5" t="n">
         <v>22400</v>
       </c>
-      <c r="H4">
-        <f>IF(AND(ISNUMBER(G4),ISNUMBER(F4)),ROUND(G4*F4/1000000,3),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="J5">
+        <f>IF(AND(ISNUMBER(I5),ISNUMBER(H5)),ROUND(I5*H5/1000000,3),)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_ABOC_K63_ABOC</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C6" t="n">
         <v>15</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Ubᴰ 5</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>200</v>
       </c>
-      <c r="D5">
-        <f>(B5*C5*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="E5" t="n">
+      <c r="F6">
+        <f>(C6*E6*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="G6" t="n">
         <v>20</v>
       </c>
-      <c r="F5">
-        <f>(B5*C5*E5*1.1/1000)</f>
-        <v/>
-      </c>
-      <c r="G5" t="n">
+      <c r="H6">
+        <f>(C6*E6*G6*1.1/1000)</f>
+        <v/>
+      </c>
+      <c r="I6" t="n">
         <v>8851</v>
       </c>
-      <c r="H5">
-        <f>IF(AND(ISNUMBER(G5),ISNUMBER(F5)),ROUND(G5*F5/1000000,3),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="J6">
+        <f>IF(AND(ISNUMBER(I6),ISNUMBER(H6)),ROUND(I6*H6/1000000,3),)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_SMAC_K63_ABOC</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C7" t="n">
         <v>2</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Ubᴰ 2</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>200</v>
       </c>
-      <c r="D6">
-        <f>(B6*C6*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="E6" t="n">
+      <c r="F7">
+        <f>(C7*E7*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="G7" t="n">
         <v>20</v>
       </c>
-      <c r="F6">
-        <f>(B6*C6*E6*1.1/1000)</f>
-        <v/>
-      </c>
-      <c r="G6" t="n">
+      <c r="H7">
+        <f>(C7*E7*G7*1.1/1000)</f>
+        <v/>
+      </c>
+      <c r="I7" t="n">
         <v>8864</v>
       </c>
-      <c r="H6">
-        <f>IF(AND(ISNUMBER(G6),ISNUMBER(F6)),ROUND(G6*F6/1000000,3),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="J7">
+        <f>IF(AND(ISNUMBER(I7),ISNUMBER(H7)),ROUND(I7*H7/1000000,3),)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_ABOC_K63_SMAC</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C8" t="n">
         <v>9</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Ubᴰ 4</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>200</v>
       </c>
-      <c r="D7">
-        <f>(B7*C7*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="E7" t="n">
+      <c r="F8">
+        <f>(C8*E8*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="G8" t="n">
         <v>20</v>
       </c>
-      <c r="F7">
-        <f>(B7*C7*E7*1.1/1000)</f>
-        <v/>
-      </c>
-      <c r="G7" t="n">
+      <c r="H8">
+        <f>(C8*E8*G8*1.1/1000)</f>
+        <v/>
+      </c>
+      <c r="I8" t="n">
         <v>8864</v>
       </c>
-      <c r="H7">
-        <f>IF(AND(ISNUMBER(G7),ISNUMBER(F7)),ROUND(G7*F7/1000000,3),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="J8">
+        <f>IF(AND(ISNUMBER(I8),ISNUMBER(H8)),ROUND(I8*H8/1000000,3),)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K48_SMAC</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C9" t="n">
         <v>2</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Ubᴰ 1</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>200</v>
       </c>
-      <c r="D8">
-        <f>(B8*C8*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="E8" t="n">
+      <c r="F9">
+        <f>(C9*E9*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="G9" t="n">
         <v>20</v>
       </c>
-      <c r="F8">
-        <f>(B8*C8*E8*1.1/1000)</f>
-        <v/>
-      </c>
-      <c r="G8" t="n">
+      <c r="H9">
+        <f>(C9*E9*G9*1.1/1000)</f>
+        <v/>
+      </c>
+      <c r="I9" t="n">
         <v>8733</v>
       </c>
-      <c r="H8">
-        <f>IF(AND(ISNUMBER(G8),ISNUMBER(F8)),ROUND(G8*F8/1000000,3),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="J9">
+        <f>IF(AND(ISNUMBER(I9),ISNUMBER(H9)),ROUND(I9*H9/1000000,3),)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
         <is>
           <t>ubi_ubq_1_K63_SMAC</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Ubᴰ 3</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
         <v>200</v>
       </c>
-      <c r="D9">
-        <f>(B9*C9*1.1)/2</f>
-        <v/>
-      </c>
-      <c r="E9" t="n">
+      <c r="F10">
+        <f>(C10*E10*1.1)/2</f>
+        <v/>
+      </c>
+      <c r="G10" t="n">
         <v>20</v>
       </c>
-      <c r="F9">
-        <f>(B9*C9*E9*1.1/1000)</f>
-        <v/>
-      </c>
-      <c r="G9" t="n">
+      <c r="H10">
+        <f>(C10*E10*G10*1.1/1000)</f>
+        <v/>
+      </c>
+      <c r="I10" t="n">
         <v>8733</v>
       </c>
-      <c r="H9">
-        <f>IF(AND(ISNUMBER(G9),ISNUMBER(F9)),ROUND(G9*F9/1000000,3),)</f>
+      <c r="J10">
+        <f>IF(AND(ISNUMBER(I10),ISNUMBER(H10)),ROUND(I10*H10/1000000,3),)</f>
         <v/>
       </c>
     </row>
@@ -1459,7 +1564,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="14" customWidth="1" min="3" max="3"/>
@@ -1481,11 +1586,11 @@
       <c r="C2" s="5" t="n"/>
       <c r="E2" s="6" t="inlineStr">
         <is>
-          <t>Base Reagent</t>
+          <t>Enzyme</t>
         </is>
       </c>
       <c r="F2" s="7">
-        <f>'Base Reagent Counts'!A2</f>
+        <f>'Base Reagent Counts'!B3</f>
         <v/>
       </c>
       <c r="G2" s="5" t="inlineStr">
@@ -1495,11 +1600,11 @@
       </c>
       <c r="J2" s="6" t="inlineStr">
         <is>
-          <t>Base Reagent</t>
+          <t>Donor: Ubᴰ 1</t>
         </is>
       </c>
       <c r="K2" s="7">
-        <f>'Base Reagent Counts'!A5</f>
+        <f>'Base Reagent Counts'!B9</f>
         <v/>
       </c>
       <c r="L2" s="5" t="inlineStr">
@@ -1523,7 +1628,7 @@
         </is>
       </c>
       <c r="F3" s="11">
-        <f>'Base Reagent Counts'!D2</f>
+        <f>'Base Reagent Counts'!F3</f>
         <v/>
       </c>
       <c r="G3" s="12" t="n"/>
@@ -1533,7 +1638,7 @@
         </is>
       </c>
       <c r="K3" s="11">
-        <f>'Base Reagent Counts'!D5</f>
+        <f>'Base Reagent Counts'!F9</f>
         <v/>
       </c>
       <c r="L3" s="12" t="n"/>
@@ -1553,7 +1658,7 @@
         </is>
       </c>
       <c r="F4" s="11">
-        <f>'Base Reagent Counts'!F2</f>
+        <f>'Base Reagent Counts'!H3</f>
         <v/>
       </c>
       <c r="G4" s="12" t="n"/>
@@ -1563,7 +1668,7 @@
         </is>
       </c>
       <c r="K4" s="11">
-        <f>'Base Reagent Counts'!F5</f>
+        <f>'Base Reagent Counts'!H9</f>
         <v/>
       </c>
       <c r="L4" s="12" t="n"/>
@@ -1910,11 +2015,11 @@
     <row r="20">
       <c r="E20" s="6" t="inlineStr">
         <is>
-          <t>Base Reagent</t>
+          <t>Enzyme</t>
         </is>
       </c>
       <c r="F20" s="7">
-        <f>'Base Reagent Counts'!A3</f>
+        <f>'Base Reagent Counts'!B4</f>
         <v/>
       </c>
       <c r="G20" s="5" t="inlineStr">
@@ -1924,11 +2029,11 @@
       </c>
       <c r="J20" s="6" t="inlineStr">
         <is>
-          <t>Base Reagent</t>
+          <t>Donor: Ubᴰ 2</t>
         </is>
       </c>
       <c r="K20" s="7">
-        <f>'Base Reagent Counts'!A6</f>
+        <f>'Base Reagent Counts'!B7</f>
         <v/>
       </c>
       <c r="L20" s="5" t="inlineStr">
@@ -1944,7 +2049,7 @@
         </is>
       </c>
       <c r="F21" s="11">
-        <f>'Base Reagent Counts'!D3</f>
+        <f>'Base Reagent Counts'!F4</f>
         <v/>
       </c>
       <c r="G21" s="12" t="n"/>
@@ -1954,7 +2059,7 @@
         </is>
       </c>
       <c r="K21" s="11">
-        <f>'Base Reagent Counts'!D6</f>
+        <f>'Base Reagent Counts'!F7</f>
         <v/>
       </c>
       <c r="L21" s="12" t="n"/>
@@ -1966,7 +2071,7 @@
         </is>
       </c>
       <c r="F22" s="11">
-        <f>'Base Reagent Counts'!F3</f>
+        <f>'Base Reagent Counts'!H4</f>
         <v/>
       </c>
       <c r="G22" s="12" t="n"/>
@@ -1976,7 +2081,7 @@
         </is>
       </c>
       <c r="K22" s="11">
-        <f>'Base Reagent Counts'!F6</f>
+        <f>'Base Reagent Counts'!H7</f>
         <v/>
       </c>
       <c r="L22" s="12" t="n"/>
@@ -2274,11 +2379,11 @@
     <row r="38">
       <c r="E38" s="6" t="inlineStr">
         <is>
-          <t>Base Reagent</t>
+          <t>Enzyme</t>
         </is>
       </c>
       <c r="F38" s="7">
-        <f>'Base Reagent Counts'!A4</f>
+        <f>'Base Reagent Counts'!B5</f>
         <v/>
       </c>
       <c r="G38" s="5" t="inlineStr">
@@ -2288,11 +2393,11 @@
       </c>
       <c r="J38" s="6" t="inlineStr">
         <is>
-          <t>Base Reagent</t>
+          <t>Donor: Ubᴰ 3</t>
         </is>
       </c>
       <c r="K38" s="7">
-        <f>'Base Reagent Counts'!A7</f>
+        <f>'Base Reagent Counts'!B10</f>
         <v/>
       </c>
       <c r="L38" s="5" t="inlineStr">
@@ -2308,7 +2413,7 @@
         </is>
       </c>
       <c r="F39" s="11">
-        <f>'Base Reagent Counts'!D4</f>
+        <f>'Base Reagent Counts'!F5</f>
         <v/>
       </c>
       <c r="G39" s="12" t="n"/>
@@ -2318,7 +2423,7 @@
         </is>
       </c>
       <c r="K39" s="11">
-        <f>'Base Reagent Counts'!D7</f>
+        <f>'Base Reagent Counts'!F10</f>
         <v/>
       </c>
       <c r="L39" s="12" t="n"/>
@@ -2330,7 +2435,7 @@
         </is>
       </c>
       <c r="F40" s="11">
-        <f>'Base Reagent Counts'!F4</f>
+        <f>'Base Reagent Counts'!H5</f>
         <v/>
       </c>
       <c r="G40" s="12" t="n"/>
@@ -2340,7 +2445,7 @@
         </is>
       </c>
       <c r="K40" s="11">
-        <f>'Base Reagent Counts'!F7</f>
+        <f>'Base Reagent Counts'!H10</f>
         <v/>
       </c>
       <c r="L40" s="12" t="n"/>
@@ -2638,11 +2743,11 @@
     <row r="56">
       <c r="J56" s="6" t="inlineStr">
         <is>
-          <t>Base Reagent</t>
+          <t>Donor: Ubᴰ 4</t>
         </is>
       </c>
       <c r="K56" s="7">
-        <f>'Base Reagent Counts'!A8</f>
+        <f>'Base Reagent Counts'!B8</f>
         <v/>
       </c>
       <c r="L56" s="5" t="inlineStr">
@@ -2658,7 +2763,7 @@
         </is>
       </c>
       <c r="K57" s="11">
-        <f>'Base Reagent Counts'!D8</f>
+        <f>'Base Reagent Counts'!F8</f>
         <v/>
       </c>
       <c r="L57" s="12" t="n"/>
@@ -2670,7 +2775,7 @@
         </is>
       </c>
       <c r="K58" s="11">
-        <f>'Base Reagent Counts'!F8</f>
+        <f>'Base Reagent Counts'!H8</f>
         <v/>
       </c>
       <c r="L58" s="12" t="n"/>
@@ -2829,11 +2934,11 @@
     <row r="74">
       <c r="J74" s="6" t="inlineStr">
         <is>
-          <t>Base Reagent</t>
+          <t>Donor: Ubᴰ 5</t>
         </is>
       </c>
       <c r="K74" s="7">
-        <f>'Base Reagent Counts'!A9</f>
+        <f>'Base Reagent Counts'!B6</f>
         <v/>
       </c>
       <c r="L74" s="5" t="inlineStr">
@@ -2849,7 +2954,7 @@
         </is>
       </c>
       <c r="K75" s="11">
-        <f>'Base Reagent Counts'!D9</f>
+        <f>'Base Reagent Counts'!F6</f>
         <v/>
       </c>
       <c r="L75" s="12" t="n"/>
@@ -2861,7 +2966,7 @@
         </is>
       </c>
       <c r="K76" s="11">
-        <f>'Base Reagent Counts'!F9</f>
+        <f>'Base Reagent Counts'!H6</f>
         <v/>
       </c>
       <c r="L76" s="12" t="n"/>
@@ -3027,13 +3132,29 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K14"/>
+  <dimension ref="B2:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="9" customWidth="1" min="9" max="9"/>
+    <col width="7" customWidth="1" min="10" max="10"/>
+    <col width="13" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="21" customWidth="1" min="15" max="15"/>
+  </cols>
   <sheetData>
     <row r="2">
       <c r="B2" s="27" t="inlineStr">
@@ -3043,42 +3164,67 @@
       </c>
       <c r="C2" s="27" t="inlineStr">
         <is>
-          <t>Acceptor</t>
+          <t>Acceptor No.</t>
         </is>
       </c>
       <c r="D2" s="27" t="inlineStr">
         <is>
+          <t>Dimer Linkage</t>
+        </is>
+      </c>
+      <c r="E2" s="27" t="inlineStr">
+        <is>
+          <t>Proximal Ub K48</t>
+        </is>
+      </c>
+      <c r="F2" s="27" t="inlineStr">
+        <is>
+          <t>Proximal Ub K63</t>
+        </is>
+      </c>
+      <c r="G2" s="27" t="inlineStr">
+        <is>
+          <t>Distal Ub K48</t>
+        </is>
+      </c>
+      <c r="H2" s="27" t="inlineStr">
+        <is>
+          <t>Distal Ub K63</t>
+        </is>
+      </c>
+      <c r="I2" s="27" t="inlineStr">
+        <is>
+          <t>MW (Da)</t>
+        </is>
+      </c>
+      <c r="J2" s="27" t="inlineStr">
+        <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>No.</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>linkage</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>proximal Ub K48</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>proximal Ub K63</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>distal Ub K48</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>distal Ub K63</t>
+      <c r="K2" s="27" t="inlineStr">
+        <is>
+          <t>nmol / well</t>
+        </is>
+      </c>
+      <c r="L2" s="27" t="inlineStr">
+        <is>
+          <t>Total nmol</t>
+        </is>
+      </c>
+      <c r="M2" s="27" t="inlineStr">
+        <is>
+          <t>Stock Conc. (uM)</t>
+        </is>
+      </c>
+      <c r="N2" s="27" t="inlineStr">
+        <is>
+          <t>Volume / well</t>
+        </is>
+      </c>
+      <c r="O2" s="27" t="inlineStr">
+        <is>
+          <t>Total Volume needed</t>
         </is>
       </c>
     </row>
@@ -3088,41 +3234,57 @@
       </c>
       <c r="C3" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_1ubq-2-(&lt;K48_SMAC&gt;&lt;K63_ABOC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D3" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
           <t>Ub₂ᴬ 9</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="D3" s="28" t="inlineStr">
         <is>
           <t>K48</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="E3" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="F3" s="28" t="inlineStr">
         <is>
           <t>K</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="G3" s="28" t="inlineStr">
         <is>
           <t>Smac</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="H3" s="28" t="inlineStr">
         <is>
           <t>Aboc</t>
         </is>
+      </c>
+      <c r="I3" s="28" t="n">
+        <v>18372</v>
+      </c>
+      <c r="J3" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L3" s="28">
+        <f>J3*K3</f>
+        <v/>
+      </c>
+      <c r="M3" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N3" s="28">
+        <f>ROUND(K3/M3*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O3" s="28">
+        <f>ROUND(L3/M3*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -3131,41 +3293,57 @@
       </c>
       <c r="C4" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_1ubq-2-(&lt;K48_ABOC&gt;&lt;K63_SMAC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D4" s="28" t="n">
+          <t>Ub₂ᴬ 10</t>
+        </is>
+      </c>
+      <c r="D4" s="28" t="inlineStr">
+        <is>
+          <t>K48</t>
+        </is>
+      </c>
+      <c r="E4" s="28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" s="28" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="G4" s="28" t="inlineStr">
+        <is>
+          <t>Aboc</t>
+        </is>
+      </c>
+      <c r="H4" s="28" t="inlineStr">
+        <is>
+          <t>Smac</t>
+        </is>
+      </c>
+      <c r="I4" s="28" t="n">
+        <v>18372</v>
+      </c>
+      <c r="J4" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Ub₂ᴬ 10</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>K48</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Aboc</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Smac</t>
-        </is>
+      <c r="K4" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L4" s="28">
+        <f>J4*K4</f>
+        <v/>
+      </c>
+      <c r="M4" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N4" s="28">
+        <f>ROUND(K4/M4*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O4" s="28">
+        <f>ROUND(L4/M4*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -3174,41 +3352,57 @@
       </c>
       <c r="C5" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_1ubq-2-(&lt;K48_ABOC&gt;&lt;K63_ABOC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D5" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
           <t>Ub₂ᴬ 11</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="D5" s="28" t="inlineStr">
         <is>
           <t>K48</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="E5" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="F5" s="28" t="inlineStr">
         <is>
           <t>K</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="G5" s="28" t="inlineStr">
         <is>
           <t>Aboc</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="H5" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="I5" s="28" t="n">
+        <v>18360</v>
+      </c>
+      <c r="J5" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" s="28">
+        <f>J5*K5</f>
+        <v/>
+      </c>
+      <c r="M5" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N5" s="28">
+        <f>ROUND(K5/M5*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O5" s="28">
+        <f>ROUND(L5/M5*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -3217,41 +3411,57 @@
       </c>
       <c r="C6" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_1ubq-2-(&lt;K48_SMAC&gt;)&gt;&lt;K63_ABOC&gt;)</t>
-        </is>
-      </c>
-      <c r="D6" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
           <t>Ub₂ᴬ 12</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="D6" s="28" t="inlineStr">
         <is>
           <t>K48</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="E6" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="F6" s="28" t="inlineStr">
         <is>
           <t>Aboc</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="G6" s="28" t="inlineStr">
         <is>
           <t>Smac</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="H6" s="28" t="inlineStr">
         <is>
           <t>K</t>
         </is>
+      </c>
+      <c r="I6" s="28" t="n">
+        <v>18372</v>
+      </c>
+      <c r="J6" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L6" s="28">
+        <f>J6*K6</f>
+        <v/>
+      </c>
+      <c r="M6" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N6" s="28">
+        <f>ROUND(K6/M6*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O6" s="28">
+        <f>ROUND(L6/M6*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -3260,41 +3470,57 @@
       </c>
       <c r="C7" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_1ubq-2-(&lt;K48_SMAC&gt;&lt;K63_ABOC&gt;)&gt;&lt;K63_ABOC&gt;)</t>
-        </is>
-      </c>
-      <c r="D7" s="28" t="n">
+          <t>Ub₂ᴬ 13</t>
+        </is>
+      </c>
+      <c r="D7" s="28" t="inlineStr">
+        <is>
+          <t>K48</t>
+        </is>
+      </c>
+      <c r="E7" s="28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" s="28" t="inlineStr">
+        <is>
+          <t>Aboc</t>
+        </is>
+      </c>
+      <c r="G7" s="28" t="inlineStr">
+        <is>
+          <t>Smac</t>
+        </is>
+      </c>
+      <c r="H7" s="28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" s="28" t="n">
+        <v>18504</v>
+      </c>
+      <c r="J7" s="28" t="n">
         <v>8</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Ub₂ᴬ 13</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>K48</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Aboc</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Smac</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="K7" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L7" s="28">
+        <f>J7*K7</f>
+        <v/>
+      </c>
+      <c r="M7" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N7" s="28">
+        <f>ROUND(K7/M7*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O7" s="28">
+        <f>ROUND(L7/M7*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -3303,41 +3529,57 @@
       </c>
       <c r="C8" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_1ubq-2-(&lt;K48_ABOC&gt;&lt;K63_SMAC&gt;)&gt;&lt;K63_ABOC&gt;)</t>
-        </is>
-      </c>
-      <c r="D8" s="28" t="n">
+          <t>Ub₂ᴬ 14</t>
+        </is>
+      </c>
+      <c r="D8" s="28" t="inlineStr">
+        <is>
+          <t>K48</t>
+        </is>
+      </c>
+      <c r="E8" s="28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" s="28" t="inlineStr">
+        <is>
+          <t>Aboc</t>
+        </is>
+      </c>
+      <c r="G8" s="28" t="inlineStr">
+        <is>
+          <t>Aboc</t>
+        </is>
+      </c>
+      <c r="H8" s="28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" s="28" t="n">
+        <v>18504</v>
+      </c>
+      <c r="J8" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Ub₂ᴬ 14</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>K48</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Aboc</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Aboc</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="K8" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L8" s="28">
+        <f>J8*K8</f>
+        <v/>
+      </c>
+      <c r="M8" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N8" s="28">
+        <f>ROUND(K8/M8*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O8" s="28">
+        <f>ROUND(L8/M8*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -3346,41 +3588,57 @@
       </c>
       <c r="C9" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K63_1ubq-2-(&lt;K48_SMAC&gt;&lt;K63_ABOC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D9" s="28" t="n">
+          <t>Ub₂ᴬ 15</t>
+        </is>
+      </c>
+      <c r="D9" s="28" t="inlineStr">
+        <is>
+          <t>K63</t>
+        </is>
+      </c>
+      <c r="E9" s="28" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="F9" s="28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" s="28" t="inlineStr">
+        <is>
+          <t>Smac</t>
+        </is>
+      </c>
+      <c r="H9" s="28" t="inlineStr">
+        <is>
+          <t>Aboc</t>
+        </is>
+      </c>
+      <c r="I9" s="28" t="n">
+        <v>18372</v>
+      </c>
+      <c r="J9" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Ub₂ᴬ 15</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>K63</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Smac</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Aboc</t>
-        </is>
+      <c r="K9" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L9" s="28">
+        <f>J9*K9</f>
+        <v/>
+      </c>
+      <c r="M9" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N9" s="28">
+        <f>ROUND(K9/M9*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O9" s="28">
+        <f>ROUND(L9/M9*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -3389,41 +3647,57 @@
       </c>
       <c r="C10" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K63_1ubq-2-(&lt;K48_ABOC&gt;&lt;K63_SMAC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D10" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
           <t>Ub₂ᴬ 16</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="D10" s="28" t="inlineStr">
         <is>
           <t>K63</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="E10" s="28" t="inlineStr">
         <is>
           <t>K</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="F10" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="G10" s="28" t="inlineStr">
         <is>
           <t>Aboc</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="H10" s="28" t="inlineStr">
         <is>
           <t>Smac</t>
         </is>
+      </c>
+      <c r="I10" s="28" t="n">
+        <v>18372</v>
+      </c>
+      <c r="J10" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" s="28">
+        <f>J10*K10</f>
+        <v/>
+      </c>
+      <c r="M10" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N10" s="28">
+        <f>ROUND(K10/M10*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O10" s="28">
+        <f>ROUND(L10/M10*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -3432,41 +3706,57 @@
       </c>
       <c r="C11" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K63_1ubq-2-(&lt;K48_ABOC&gt;&lt;K63_ABOC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D11" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
           <t>Ub₂ᴬ 17</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="D11" s="28" t="inlineStr">
         <is>
           <t>K63</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="E11" s="28" t="inlineStr">
         <is>
           <t>K</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="F11" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="G11" s="28" t="inlineStr">
         <is>
           <t>Aboc</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="H11" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="I11" s="28" t="n">
+        <v>18360</v>
+      </c>
+      <c r="J11" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L11" s="28">
+        <f>J11*K11</f>
+        <v/>
+      </c>
+      <c r="M11" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N11" s="28">
+        <f>ROUND(K11/M11*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O11" s="28">
+        <f>ROUND(L11/M11*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -3475,41 +3765,57 @@
       </c>
       <c r="C12" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_ABOC&gt;&lt;K63_1ubq-2-(&lt;K63_SMAC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D12" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
           <t>Ub₂ᴬ 18</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="D12" s="28" t="inlineStr">
         <is>
           <t>K63</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="E12" s="28" t="inlineStr">
         <is>
           <t>Aboc</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="F12" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="G12" s="28" t="inlineStr">
         <is>
           <t>K</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="H12" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="I12" s="28" t="n">
+        <v>18372</v>
+      </c>
+      <c r="J12" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L12" s="28">
+        <f>J12*K12</f>
+        <v/>
+      </c>
+      <c r="M12" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N12" s="28">
+        <f>ROUND(K12/M12*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O12" s="28">
+        <f>ROUND(L12/M12*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -3518,41 +3824,57 @@
       </c>
       <c r="C13" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_ABOC&gt;&lt;K63_1ubq-2-(&lt;K48_SMAC&gt;&lt;K63_ABOC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D13" s="28" t="n">
+          <t>Ub₂ᴬ 19</t>
+        </is>
+      </c>
+      <c r="D13" s="28" t="inlineStr">
+        <is>
+          <t>K63</t>
+        </is>
+      </c>
+      <c r="E13" s="28" t="inlineStr">
+        <is>
+          <t>Aboc</t>
+        </is>
+      </c>
+      <c r="F13" s="28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" s="28" t="inlineStr">
+        <is>
+          <t>Smac</t>
+        </is>
+      </c>
+      <c r="H13" s="28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" s="28" t="n">
+        <v>18504</v>
+      </c>
+      <c r="J13" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Ub₂ᴬ 19</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>K63</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Aboc</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Smac</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="K13" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L13" s="28">
+        <f>J13*K13</f>
+        <v/>
+      </c>
+      <c r="M13" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N13" s="28">
+        <f>ROUND(K13/M13*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O13" s="28">
+        <f>ROUND(L13/M13*1000,2)</f>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -3561,41 +3883,57 @@
       </c>
       <c r="C14" s="28" t="inlineStr">
         <is>
-          <t>his-GG-1ubq-1-(&lt;K48_ABOC&gt;&lt;K63_1ubq-2-(&lt;K48_ABOC&gt;&lt;K63_SMAC&gt;)&gt;)</t>
-        </is>
-      </c>
-      <c r="D14" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
           <t>Ub₂ᴬ 20</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="D14" s="28" t="inlineStr">
         <is>
           <t>K63</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="E14" s="28" t="inlineStr">
         <is>
           <t>Aboc</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="F14" s="28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="G14" s="28" t="inlineStr">
         <is>
           <t>Aboc</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="H14" s="28" t="inlineStr">
         <is>
           <t>Smac</t>
         </is>
+      </c>
+      <c r="I14" s="28" t="n">
+        <v>18504</v>
+      </c>
+      <c r="J14" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="L14" s="28">
+        <f>J14*K14</f>
+        <v/>
+      </c>
+      <c r="M14" s="28" t="n">
+        <v>20</v>
+      </c>
+      <c r="N14" s="28">
+        <f>ROUND(K14/M14*1000,2)</f>
+        <v/>
+      </c>
+      <c r="O14" s="28">
+        <f>ROUND(L14/M14*1000,2)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>